<commit_message>
feat：fix obby bug and pet language bug
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/Language_多语言表.xlsx
+++ b/pet-simulator/Excel/Language_多语言表.xlsx
@@ -4842,7 +4842,7 @@
     <t>Task_Info_20</t>
   </si>
   <si>
-    <t>Hatch {0} pets of rare or above from the undersea egg</t>
+    <t>Hatch {0} pets of Rare or above rarity</t>
   </si>
   <si>
     <t>从海底蛋中孵化{0}只稀有以上的宠物</t>
@@ -9824,8 +9824,8 @@
   <sheetPr/>
   <dimension ref="A1:T1038"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A590" workbookViewId="0">
-      <selection activeCell="F605" sqref="F605"/>
+    <sheetView tabSelected="1" topLeftCell="A592" workbookViewId="0">
+      <selection activeCell="G604" sqref="G604"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.125" defaultRowHeight="16.5"/>

</xml_diff>

<commit_message>
feat: update pet UI
根据figma修改petUI
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/Language_多语言表.xlsx
+++ b/pet-simulator/Excel/Language_多语言表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Project\Edit\DragonVerse\pet-simulator\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7286D337-E317-474A-A51C-C669542022C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8E9360-0D01-405E-B345-EF4E8276E791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5243" uniqueCount="2972">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5248" uniqueCount="2975">
   <si>
     <t>int</t>
   </si>
@@ -8445,12 +8445,6 @@
     <t>CurrentRoomId</t>
   </si>
   <si>
-    <t>Room ID: {0}</t>
-  </si>
-  <si>
-    <t>房间ID：{0}</t>
-  </si>
-  <si>
     <t>JumpGameFailed</t>
   </si>
   <si>
@@ -8555,9 +8549,6 @@
   </si>
   <si>
     <t>Stamina mechanism</t>
-  </si>
-  <si>
-    <t>Current room id:{0}</t>
   </si>
   <si>
     <t>Switch Room Failed!</t>
@@ -9034,6 +9025,30 @@
   </si>
   <si>
     <t>Switch Room Failed!</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Room ID: {0}</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Switch room</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>房间ID：{0}</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>开蛋！</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Open!</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>OpenEgg</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -9649,10 +9664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T1047"/>
+  <dimension ref="A1:T1048"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A953" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1038" sqref="A1038"/>
+    <sheetView tabSelected="1" topLeftCell="A1010" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1041" sqref="F1041"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.125" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -14965,19 +14980,19 @@
         <v>257</v>
       </c>
       <c r="B261" s="31" t="s">
-        <v>2907</v>
+        <v>2904</v>
       </c>
       <c r="C261" s="3" t="s">
-        <v>2857</v>
+        <v>2854</v>
       </c>
       <c r="D261" s="4" t="s">
-        <v>2849</v>
+        <v>2846</v>
       </c>
       <c r="E261" s="3" t="s">
-        <v>2857</v>
+        <v>2854</v>
       </c>
       <c r="F261" s="3" t="s">
-        <v>2857</v>
+        <v>2854</v>
       </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.35">
@@ -14988,16 +15003,16 @@
         <v>581</v>
       </c>
       <c r="C262" s="3" t="s">
-        <v>2861</v>
+        <v>2858</v>
       </c>
       <c r="D262" s="4" t="s">
-        <v>2905</v>
+        <v>2902</v>
       </c>
       <c r="E262" s="3" t="s">
-        <v>2861</v>
+        <v>2858</v>
       </c>
       <c r="F262" s="3" t="s">
-        <v>2861</v>
+        <v>2858</v>
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.35">
@@ -15008,16 +15023,16 @@
         <v>582</v>
       </c>
       <c r="C263" s="33" t="s">
-        <v>2932</v>
+        <v>2929</v>
       </c>
       <c r="D263" s="35" t="s">
-        <v>2931</v>
+        <v>2928</v>
       </c>
       <c r="E263" s="3" t="s">
-        <v>2932</v>
+        <v>2929</v>
       </c>
       <c r="F263" s="3" t="s">
-        <v>2932</v>
+        <v>2929</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.35">
@@ -15028,16 +15043,16 @@
         <v>583</v>
       </c>
       <c r="C264" s="33" t="s">
-        <v>2933</v>
+        <v>2930</v>
       </c>
       <c r="D264" s="4" t="s">
-        <v>2927</v>
+        <v>2924</v>
       </c>
       <c r="E264" s="3" t="s">
-        <v>2933</v>
+        <v>2930</v>
       </c>
       <c r="F264" s="3" t="s">
-        <v>2933</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.35">
@@ -15048,16 +15063,16 @@
         <v>584</v>
       </c>
       <c r="C265" s="33" t="s">
-        <v>2938</v>
+        <v>2935</v>
       </c>
       <c r="D265" s="35" t="s">
+        <v>2932</v>
+      </c>
+      <c r="E265" s="3" t="s">
         <v>2935</v>
       </c>
-      <c r="E265" s="3" t="s">
-        <v>2938</v>
-      </c>
       <c r="F265" s="3" t="s">
-        <v>2938</v>
+        <v>2935</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.35">
@@ -15068,16 +15083,16 @@
         <v>585</v>
       </c>
       <c r="C266" s="33" t="s">
-        <v>2946</v>
+        <v>2943</v>
       </c>
       <c r="D266" s="35" t="s">
-        <v>2942</v>
+        <v>2939</v>
       </c>
       <c r="E266" s="3" t="s">
-        <v>2946</v>
+        <v>2943</v>
       </c>
       <c r="F266" s="3" t="s">
-        <v>2946</v>
+        <v>2943</v>
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.35">
@@ -15088,16 +15103,16 @@
         <v>586</v>
       </c>
       <c r="C267" s="3" t="s">
-        <v>2912</v>
+        <v>2909</v>
       </c>
       <c r="D267" s="35" t="s">
-        <v>2948</v>
+        <v>2945</v>
       </c>
       <c r="E267" s="3" t="s">
-        <v>2912</v>
+        <v>2909</v>
       </c>
       <c r="F267" s="3" t="s">
-        <v>2912</v>
+        <v>2909</v>
       </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.35">
@@ -15328,7 +15343,7 @@
         <v>620</v>
       </c>
       <c r="C279" s="6" t="s">
-        <v>2819</v>
+        <v>2817</v>
       </c>
       <c r="D279" s="1" t="s">
         <v>621</v>
@@ -15396,7 +15411,7 @@
         <v>627</v>
       </c>
       <c r="C281" s="6" t="s">
-        <v>2820</v>
+        <v>2818</v>
       </c>
       <c r="D281" s="1" t="s">
         <v>629</v>
@@ -15430,7 +15445,7 @@
         <v>630</v>
       </c>
       <c r="C282" s="6" t="s">
-        <v>2821</v>
+        <v>2819</v>
       </c>
       <c r="D282" s="1" t="s">
         <v>632</v>
@@ -15875,7 +15890,7 @@
         <v>699</v>
       </c>
       <c r="D302" s="6" t="s">
-        <v>2822</v>
+        <v>2820</v>
       </c>
       <c r="E302" s="3" t="s">
         <v>700</v>
@@ -21404,16 +21419,16 @@
         <v>1458</v>
       </c>
       <c r="C552" s="3" t="s">
-        <v>2913</v>
+        <v>2910</v>
       </c>
       <c r="D552" s="16" t="s">
-        <v>2949</v>
+        <v>2946</v>
       </c>
       <c r="E552" s="3" t="s">
-        <v>2913</v>
+        <v>2910</v>
       </c>
       <c r="F552" s="3" t="s">
-        <v>2913</v>
+        <v>2910</v>
       </c>
     </row>
     <row r="553" spans="1:8" ht="33" x14ac:dyDescent="0.35">
@@ -21524,19 +21539,19 @@
         <v>1474</v>
       </c>
       <c r="C558" s="33" t="s">
-        <v>2845</v>
+        <v>2842</v>
       </c>
       <c r="D558" s="31" t="s">
-        <v>2847</v>
+        <v>2844</v>
       </c>
       <c r="E558" s="3" t="s">
-        <v>2845</v>
+        <v>2842</v>
       </c>
       <c r="F558" s="3" t="s">
-        <v>2845</v>
+        <v>2842</v>
       </c>
       <c r="H558" s="31" t="s">
-        <v>2846</v>
+        <v>2843</v>
       </c>
     </row>
     <row r="559" spans="1:8" x14ac:dyDescent="0.35">
@@ -21547,19 +21562,19 @@
         <v>1475</v>
       </c>
       <c r="C559" s="33" t="s">
-        <v>2853</v>
+        <v>2850</v>
       </c>
       <c r="D559" s="31" t="s">
-        <v>2852</v>
+        <v>2849</v>
       </c>
       <c r="E559" s="3" t="s">
-        <v>2853</v>
+        <v>2850</v>
       </c>
       <c r="F559" s="3" t="s">
-        <v>2853</v>
+        <v>2850</v>
       </c>
       <c r="H559" s="31" t="s">
-        <v>2854</v>
+        <v>2851</v>
       </c>
     </row>
     <row r="560" spans="1:8" x14ac:dyDescent="0.35">
@@ -21570,19 +21585,19 @@
         <v>1476</v>
       </c>
       <c r="C560" s="33" t="s">
-        <v>2855</v>
+        <v>2852</v>
       </c>
       <c r="D560" s="31" t="s">
-        <v>2924</v>
+        <v>2921</v>
       </c>
       <c r="E560" s="3" t="s">
-        <v>2855</v>
+        <v>2852</v>
       </c>
       <c r="F560" s="3" t="s">
-        <v>2855</v>
+        <v>2852</v>
       </c>
       <c r="H560" s="31" t="s">
-        <v>2856</v>
+        <v>2853</v>
       </c>
     </row>
     <row r="561" spans="1:8" x14ac:dyDescent="0.35">
@@ -21593,19 +21608,19 @@
         <v>1477</v>
       </c>
       <c r="C561" s="33" t="s">
-        <v>2863</v>
+        <v>2860</v>
       </c>
       <c r="D561" s="31" t="s">
-        <v>2926</v>
+        <v>2923</v>
       </c>
       <c r="E561" s="3" t="s">
-        <v>2863</v>
+        <v>2860</v>
       </c>
       <c r="F561" s="3" t="s">
-        <v>2863</v>
+        <v>2860</v>
       </c>
       <c r="H561" s="31" t="s">
-        <v>2864</v>
+        <v>2861</v>
       </c>
     </row>
     <row r="562" spans="1:8" x14ac:dyDescent="0.35">
@@ -21616,19 +21631,19 @@
         <v>1478</v>
       </c>
       <c r="C562" s="33" t="s">
-        <v>2865</v>
+        <v>2862</v>
       </c>
       <c r="D562" s="31" t="s">
-        <v>2934</v>
+        <v>2931</v>
       </c>
       <c r="E562" s="3" t="s">
-        <v>2865</v>
+        <v>2862</v>
       </c>
       <c r="F562" s="3" t="s">
-        <v>2865</v>
+        <v>2862</v>
       </c>
       <c r="H562" s="31" t="s">
-        <v>2866</v>
+        <v>2863</v>
       </c>
     </row>
     <row r="563" spans="1:8" x14ac:dyDescent="0.35">
@@ -21639,19 +21654,19 @@
         <v>1479</v>
       </c>
       <c r="C563" s="33" t="s">
-        <v>2867</v>
+        <v>2864</v>
       </c>
       <c r="D563" s="31" t="s">
-        <v>2941</v>
+        <v>2938</v>
       </c>
       <c r="E563" s="3" t="s">
-        <v>2908</v>
+        <v>2905</v>
       </c>
       <c r="F563" s="3" t="s">
-        <v>2908</v>
+        <v>2905</v>
       </c>
       <c r="H563" s="31" t="s">
-        <v>2868</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="564" spans="1:8" x14ac:dyDescent="0.35">
@@ -21662,19 +21677,19 @@
         <v>1480</v>
       </c>
       <c r="C564" s="33" t="s">
-        <v>2869</v>
+        <v>2866</v>
       </c>
       <c r="D564" s="31" t="s">
-        <v>2947</v>
+        <v>2944</v>
       </c>
       <c r="E564" s="33" t="s">
-        <v>2870</v>
+        <v>2867</v>
       </c>
       <c r="F564" s="3" t="s">
-        <v>2869</v>
+        <v>2866</v>
       </c>
       <c r="H564" s="31" t="s">
-        <v>2870</v>
+        <v>2867</v>
       </c>
     </row>
     <row r="565" spans="1:8" x14ac:dyDescent="0.35">
@@ -21685,19 +21700,19 @@
         <v>1481</v>
       </c>
       <c r="C565" s="33" t="s">
-        <v>2871</v>
+        <v>2868</v>
       </c>
       <c r="D565" s="1" t="s">
-        <v>2950</v>
+        <v>2947</v>
       </c>
       <c r="E565" s="3" t="s">
-        <v>2871</v>
+        <v>2868</v>
       </c>
       <c r="F565" s="3" t="s">
-        <v>2871</v>
+        <v>2868</v>
       </c>
       <c r="H565" s="31" t="s">
-        <v>2872</v>
+        <v>2869</v>
       </c>
     </row>
     <row r="566" spans="1:8" x14ac:dyDescent="0.35">
@@ -21708,19 +21723,19 @@
         <v>1482</v>
       </c>
       <c r="C566" s="33" t="s">
-        <v>2873</v>
+        <v>2870</v>
       </c>
       <c r="D566" s="31" t="s">
-        <v>2953</v>
+        <v>2950</v>
       </c>
       <c r="E566" s="3" t="s">
-        <v>2873</v>
+        <v>2870</v>
       </c>
       <c r="F566" s="3" t="s">
-        <v>2873</v>
+        <v>2870</v>
       </c>
       <c r="H566" s="31" t="s">
-        <v>2874</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="567" spans="1:8" x14ac:dyDescent="0.35">
@@ -21731,19 +21746,19 @@
         <v>1483</v>
       </c>
       <c r="C567" s="33" t="s">
-        <v>2875</v>
+        <v>2872</v>
       </c>
       <c r="D567" s="31" t="s">
-        <v>2955</v>
+        <v>2952</v>
       </c>
       <c r="E567" s="3" t="s">
-        <v>2875</v>
+        <v>2872</v>
       </c>
       <c r="F567" s="3" t="s">
-        <v>2875</v>
+        <v>2872</v>
       </c>
       <c r="H567" s="31" t="s">
-        <v>2876</v>
+        <v>2873</v>
       </c>
     </row>
     <row r="568" spans="1:8" x14ac:dyDescent="0.35">
@@ -21754,19 +21769,19 @@
         <v>1484</v>
       </c>
       <c r="C568" s="33" t="s">
-        <v>2877</v>
+        <v>2874</v>
       </c>
       <c r="D568" s="31" t="s">
-        <v>2959</v>
+        <v>2956</v>
       </c>
       <c r="E568" s="3" t="s">
-        <v>2877</v>
+        <v>2874</v>
       </c>
       <c r="F568" s="3" t="s">
-        <v>2877</v>
+        <v>2874</v>
       </c>
       <c r="H568" s="31" t="s">
-        <v>2878</v>
+        <v>2875</v>
       </c>
     </row>
     <row r="569" spans="1:8" x14ac:dyDescent="0.35">
@@ -21777,19 +21792,19 @@
         <v>1485</v>
       </c>
       <c r="C569" s="33" t="s">
-        <v>2879</v>
+        <v>2876</v>
       </c>
       <c r="D569" s="31" t="s">
-        <v>2961</v>
+        <v>2958</v>
       </c>
       <c r="E569" s="3" t="s">
-        <v>2879</v>
+        <v>2876</v>
       </c>
       <c r="F569" s="3" t="s">
-        <v>2879</v>
+        <v>2876</v>
       </c>
       <c r="H569" s="31" t="s">
-        <v>2880</v>
+        <v>2877</v>
       </c>
     </row>
     <row r="570" spans="1:8" x14ac:dyDescent="0.35">
@@ -21800,19 +21815,19 @@
         <v>1486</v>
       </c>
       <c r="C570" s="33" t="s">
-        <v>2881</v>
+        <v>2878</v>
       </c>
       <c r="D570" s="31" t="s">
-        <v>2962</v>
+        <v>2959</v>
       </c>
       <c r="E570" s="3" t="s">
-        <v>2881</v>
+        <v>2878</v>
       </c>
       <c r="F570" s="3" t="s">
-        <v>2881</v>
+        <v>2878</v>
       </c>
       <c r="H570" s="31" t="s">
-        <v>2882</v>
+        <v>2879</v>
       </c>
     </row>
     <row r="571" spans="1:8" x14ac:dyDescent="0.35">
@@ -21823,19 +21838,19 @@
         <v>1487</v>
       </c>
       <c r="C571" s="33" t="s">
-        <v>2883</v>
+        <v>2880</v>
       </c>
       <c r="D571" s="31" t="s">
-        <v>2963</v>
+        <v>2960</v>
       </c>
       <c r="E571" s="3" t="s">
-        <v>2883</v>
+        <v>2880</v>
       </c>
       <c r="F571" s="3" t="s">
-        <v>2883</v>
+        <v>2880</v>
       </c>
       <c r="H571" s="31" t="s">
-        <v>2884</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="572" spans="1:8" x14ac:dyDescent="0.35">
@@ -21846,19 +21861,19 @@
         <v>1488</v>
       </c>
       <c r="C572" s="33" t="s">
-        <v>2885</v>
+        <v>2882</v>
       </c>
       <c r="D572" s="31" t="s">
-        <v>2964</v>
+        <v>2961</v>
       </c>
       <c r="E572" s="3" t="s">
-        <v>2885</v>
+        <v>2882</v>
       </c>
       <c r="F572" s="3" t="s">
-        <v>2885</v>
+        <v>2882</v>
       </c>
       <c r="H572" s="31" t="s">
-        <v>2886</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="573" spans="1:8" x14ac:dyDescent="0.35">
@@ -21866,22 +21881,22 @@
         <v>569</v>
       </c>
       <c r="B573" s="31" t="s">
-        <v>2887</v>
+        <v>2884</v>
       </c>
       <c r="C573" s="33" t="s">
-        <v>2888</v>
+        <v>2885</v>
       </c>
       <c r="D573" s="31" t="s">
-        <v>2965</v>
+        <v>2962</v>
       </c>
       <c r="E573" s="3" t="s">
-        <v>2888</v>
+        <v>2885</v>
       </c>
       <c r="F573" s="3" t="s">
-        <v>2888</v>
+        <v>2885</v>
       </c>
       <c r="H573" s="31" t="s">
-        <v>2889</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="574" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
@@ -22112,16 +22127,16 @@
         <v>1524</v>
       </c>
       <c r="C585" s="3" t="s">
-        <v>2860</v>
+        <v>2857</v>
       </c>
       <c r="D585" s="1" t="s">
-        <v>2848</v>
+        <v>2845</v>
       </c>
       <c r="E585" s="3" t="s">
-        <v>2860</v>
+        <v>2857</v>
       </c>
       <c r="F585" s="3" t="s">
-        <v>2860</v>
+        <v>2857</v>
       </c>
     </row>
     <row r="586" spans="1:6" ht="33" x14ac:dyDescent="0.35">
@@ -22152,16 +22167,16 @@
         <v>1528</v>
       </c>
       <c r="C587" s="3" t="s">
-        <v>2858</v>
+        <v>2855</v>
       </c>
       <c r="D587" s="1" t="s">
-        <v>2850</v>
+        <v>2847</v>
       </c>
       <c r="E587" s="3" t="s">
-        <v>2858</v>
+        <v>2855</v>
       </c>
       <c r="F587" s="3" t="s">
-        <v>2858</v>
+        <v>2855</v>
       </c>
     </row>
     <row r="588" spans="1:6" x14ac:dyDescent="0.35">
@@ -22192,16 +22207,16 @@
         <v>1532</v>
       </c>
       <c r="C589" s="3" t="s">
-        <v>2859</v>
+        <v>2856</v>
       </c>
       <c r="D589" s="1" t="s">
-        <v>2851</v>
+        <v>2848</v>
       </c>
       <c r="E589" s="3" t="s">
-        <v>2859</v>
+        <v>2856</v>
       </c>
       <c r="F589" s="3" t="s">
-        <v>2859</v>
+        <v>2856</v>
       </c>
     </row>
     <row r="590" spans="1:6" ht="33" x14ac:dyDescent="0.35">
@@ -22212,16 +22227,16 @@
         <v>1533</v>
       </c>
       <c r="C590" s="3" t="s">
-        <v>2862</v>
+        <v>2859</v>
       </c>
       <c r="D590" s="1" t="s">
-        <v>2906</v>
+        <v>2903</v>
       </c>
       <c r="E590" s="3" t="s">
-        <v>2862</v>
+        <v>2859</v>
       </c>
       <c r="F590" s="3" t="s">
-        <v>2862</v>
+        <v>2859</v>
       </c>
     </row>
     <row r="591" spans="1:6" ht="33" x14ac:dyDescent="0.35">
@@ -22232,7 +22247,7 @@
         <v>1534</v>
       </c>
       <c r="C591" s="3" t="s">
-        <v>2823</v>
+        <v>2821</v>
       </c>
       <c r="D591" s="1" t="s">
         <v>1536</v>
@@ -22272,16 +22287,16 @@
         <v>1541</v>
       </c>
       <c r="C593" s="3" t="s">
-        <v>2901</v>
+        <v>2898</v>
       </c>
       <c r="D593" s="1" t="s">
-        <v>2925</v>
+        <v>2922</v>
       </c>
       <c r="E593" s="3" t="s">
-        <v>2901</v>
+        <v>2898</v>
       </c>
       <c r="F593" s="3" t="s">
-        <v>2901</v>
+        <v>2898</v>
       </c>
     </row>
     <row r="594" spans="1:6" ht="33" x14ac:dyDescent="0.35">
@@ -22332,16 +22347,16 @@
         <v>1548</v>
       </c>
       <c r="C596" s="3" t="s">
-        <v>2902</v>
+        <v>2899</v>
       </c>
       <c r="D596" s="1" t="s">
-        <v>2928</v>
+        <v>2925</v>
       </c>
       <c r="E596" s="3" t="s">
-        <v>2902</v>
+        <v>2899</v>
       </c>
       <c r="F596" s="3" t="s">
-        <v>2902</v>
+        <v>2899</v>
       </c>
     </row>
     <row r="597" spans="1:6" ht="33" x14ac:dyDescent="0.35">
@@ -22352,16 +22367,16 @@
         <v>1549</v>
       </c>
       <c r="C597" s="3" t="s">
-        <v>2903</v>
+        <v>2900</v>
       </c>
       <c r="D597" s="1" t="s">
-        <v>2929</v>
+        <v>2926</v>
       </c>
       <c r="E597" s="3" t="s">
-        <v>2903</v>
+        <v>2900</v>
       </c>
       <c r="F597" s="3" t="s">
-        <v>2903</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="598" spans="1:6" ht="33" x14ac:dyDescent="0.35">
@@ -22372,16 +22387,16 @@
         <v>1550</v>
       </c>
       <c r="C598" s="3" t="s">
-        <v>2904</v>
+        <v>2901</v>
       </c>
       <c r="D598" s="1" t="s">
-        <v>2930</v>
+        <v>2927</v>
       </c>
       <c r="E598" s="3" t="s">
-        <v>2904</v>
+        <v>2901</v>
       </c>
       <c r="F598" s="3" t="s">
-        <v>2904</v>
+        <v>2901</v>
       </c>
     </row>
     <row r="599" spans="1:6" x14ac:dyDescent="0.35">
@@ -22412,16 +22427,16 @@
         <v>1554</v>
       </c>
       <c r="C600" s="3" t="s">
-        <v>2909</v>
+        <v>2906</v>
       </c>
       <c r="D600" s="1" t="s">
-        <v>2936</v>
+        <v>2933</v>
       </c>
       <c r="E600" s="3" t="s">
-        <v>2909</v>
+        <v>2906</v>
       </c>
       <c r="F600" s="3" t="s">
-        <v>2909</v>
+        <v>2906</v>
       </c>
     </row>
     <row r="601" spans="1:6" ht="33" x14ac:dyDescent="0.35">
@@ -22432,16 +22447,16 @@
         <v>1555</v>
       </c>
       <c r="C601" s="3" t="s">
-        <v>2939</v>
+        <v>2936</v>
       </c>
       <c r="D601" s="1" t="s">
+        <v>2934</v>
+      </c>
+      <c r="E601" s="3" t="s">
         <v>2937</v>
       </c>
-      <c r="E601" s="3" t="s">
-        <v>2940</v>
-      </c>
       <c r="F601" s="3" t="s">
-        <v>2940</v>
+        <v>2937</v>
       </c>
     </row>
     <row r="602" spans="1:6" ht="33" x14ac:dyDescent="0.35">
@@ -22455,13 +22470,13 @@
         <v>1557</v>
       </c>
       <c r="D602" s="1" t="s">
-        <v>2943</v>
+        <v>2940</v>
       </c>
       <c r="E602" s="3" t="s">
-        <v>2910</v>
+        <v>2907</v>
       </c>
       <c r="F602" s="3" t="s">
-        <v>2910</v>
+        <v>2907</v>
       </c>
     </row>
     <row r="603" spans="1:6" ht="33" x14ac:dyDescent="0.35">
@@ -22475,7 +22490,7 @@
         <v>1559</v>
       </c>
       <c r="D603" s="1" t="s">
-        <v>2944</v>
+        <v>2941</v>
       </c>
       <c r="E603" s="3" t="s">
         <v>1560</v>
@@ -22495,13 +22510,13 @@
         <v>1562</v>
       </c>
       <c r="D604" s="1" t="s">
-        <v>2945</v>
+        <v>2942</v>
       </c>
       <c r="E604" s="3" t="s">
-        <v>2911</v>
+        <v>2908</v>
       </c>
       <c r="F604" s="3" t="s">
-        <v>2911</v>
+        <v>2908</v>
       </c>
     </row>
     <row r="605" spans="1:6" ht="33" x14ac:dyDescent="0.35">
@@ -22512,16 +22527,16 @@
         <v>1563</v>
       </c>
       <c r="C605" s="3" t="s">
-        <v>2914</v>
+        <v>2911</v>
       </c>
       <c r="D605" s="1" t="s">
-        <v>2951</v>
+        <v>2948</v>
       </c>
       <c r="E605" s="3" t="s">
-        <v>2914</v>
+        <v>2911</v>
       </c>
       <c r="F605" s="3" t="s">
-        <v>2914</v>
+        <v>2911</v>
       </c>
     </row>
     <row r="606" spans="1:6" ht="33" x14ac:dyDescent="0.35">
@@ -22532,16 +22547,16 @@
         <v>1564</v>
       </c>
       <c r="C606" s="3" t="s">
-        <v>2915</v>
+        <v>2912</v>
       </c>
       <c r="D606" s="1" t="s">
-        <v>2952</v>
+        <v>2949</v>
       </c>
       <c r="E606" s="3" t="s">
-        <v>2915</v>
+        <v>2912</v>
       </c>
       <c r="F606" s="3" t="s">
-        <v>2915</v>
+        <v>2912</v>
       </c>
     </row>
     <row r="607" spans="1:6" x14ac:dyDescent="0.35">
@@ -22572,16 +22587,16 @@
         <v>1567</v>
       </c>
       <c r="C608" s="3" t="s">
-        <v>2917</v>
+        <v>2914</v>
       </c>
       <c r="D608" s="1" t="s">
-        <v>2954</v>
+        <v>2951</v>
       </c>
       <c r="E608" s="3" t="s">
-        <v>2917</v>
+        <v>2914</v>
       </c>
       <c r="F608" s="3" t="s">
-        <v>2917</v>
+        <v>2914</v>
       </c>
     </row>
     <row r="609" spans="1:6" ht="33" x14ac:dyDescent="0.35">
@@ -22592,16 +22607,16 @@
         <v>1568</v>
       </c>
       <c r="C609" s="3" t="s">
-        <v>2918</v>
+        <v>2915</v>
       </c>
       <c r="D609" s="1" t="s">
         <v>1569</v>
       </c>
       <c r="E609" s="3" t="s">
-        <v>2918</v>
+        <v>2915</v>
       </c>
       <c r="F609" s="3" t="s">
-        <v>2918</v>
+        <v>2915</v>
       </c>
     </row>
     <row r="610" spans="1:6" ht="33" x14ac:dyDescent="0.35">
@@ -22615,7 +22630,7 @@
         <v>1571</v>
       </c>
       <c r="D610" s="1" t="s">
-        <v>2968</v>
+        <v>2965</v>
       </c>
       <c r="E610" s="3" t="s">
         <v>1571</v>
@@ -22632,16 +22647,16 @@
         <v>1572</v>
       </c>
       <c r="C611" s="3" t="s">
-        <v>2919</v>
+        <v>2916</v>
       </c>
       <c r="D611" s="1" t="s">
-        <v>2956</v>
+        <v>2953</v>
       </c>
       <c r="E611" s="3" t="s">
-        <v>2919</v>
+        <v>2916</v>
       </c>
       <c r="F611" s="3" t="s">
-        <v>2919</v>
+        <v>2916</v>
       </c>
     </row>
     <row r="612" spans="1:6" ht="33" x14ac:dyDescent="0.35">
@@ -22652,16 +22667,16 @@
         <v>1573</v>
       </c>
       <c r="C612" s="3" t="s">
-        <v>2920</v>
+        <v>2917</v>
       </c>
       <c r="D612" s="1" t="s">
-        <v>2957</v>
+        <v>2954</v>
       </c>
       <c r="E612" s="3" t="s">
-        <v>2920</v>
+        <v>2917</v>
       </c>
       <c r="F612" s="3" t="s">
-        <v>2920</v>
+        <v>2917</v>
       </c>
     </row>
     <row r="613" spans="1:6" ht="33" x14ac:dyDescent="0.35">
@@ -22672,16 +22687,16 @@
         <v>1574</v>
       </c>
       <c r="C613" s="3" t="s">
-        <v>2921</v>
+        <v>2918</v>
       </c>
       <c r="D613" s="1" t="s">
-        <v>2958</v>
+        <v>2955</v>
       </c>
       <c r="E613" s="3" t="s">
-        <v>2921</v>
+        <v>2918</v>
       </c>
       <c r="F613" s="3" t="s">
-        <v>2921</v>
+        <v>2918</v>
       </c>
     </row>
     <row r="614" spans="1:6" x14ac:dyDescent="0.35">
@@ -23135,7 +23150,7 @@
         <v>1640</v>
       </c>
       <c r="D636" s="1" t="s">
-        <v>2960</v>
+        <v>2957</v>
       </c>
       <c r="E636" s="3" t="s">
         <v>1640</v>
@@ -24612,7 +24627,7 @@
         <v>1855</v>
       </c>
       <c r="C710" s="3" t="s">
-        <v>2824</v>
+        <v>2822</v>
       </c>
       <c r="D710" s="1" t="s">
         <v>1857</v>
@@ -24632,7 +24647,7 @@
         <v>1858</v>
       </c>
       <c r="C711" s="3" t="s">
-        <v>2825</v>
+        <v>2823</v>
       </c>
       <c r="D711" s="1" t="s">
         <v>1860</v>
@@ -24812,7 +24827,7 @@
         <v>1880</v>
       </c>
       <c r="C720" s="3" t="s">
-        <v>2826</v>
+        <v>2824</v>
       </c>
       <c r="D720" s="1" t="s">
         <v>870</v>
@@ -24832,7 +24847,7 @@
         <v>1881</v>
       </c>
       <c r="C721" s="3" t="s">
-        <v>2827</v>
+        <v>2825</v>
       </c>
       <c r="D721" s="1" t="s">
         <v>1883</v>
@@ -25952,7 +25967,7 @@
         <v>2043</v>
       </c>
       <c r="C777" s="24" t="s">
-        <v>2828</v>
+        <v>2826</v>
       </c>
       <c r="D777" s="1" t="s">
         <v>2045</v>
@@ -26092,16 +26107,16 @@
         <v>2064</v>
       </c>
       <c r="C784" s="24" t="s">
-        <v>2916</v>
+        <v>2913</v>
       </c>
       <c r="D784" s="31" t="s">
-        <v>2966</v>
+        <v>2963</v>
       </c>
       <c r="E784" s="24" t="s">
-        <v>2916</v>
+        <v>2913</v>
       </c>
       <c r="F784" s="24" t="s">
-        <v>2916</v>
+        <v>2913</v>
       </c>
     </row>
     <row r="785" spans="1:6" ht="17.25" x14ac:dyDescent="0.35">
@@ -26132,16 +26147,16 @@
         <v>2068</v>
       </c>
       <c r="C786" s="34" t="s">
-        <v>2923</v>
+        <v>2920</v>
       </c>
       <c r="D786" s="31" t="s">
-        <v>2967</v>
+        <v>2964</v>
       </c>
       <c r="E786" s="24" t="s">
-        <v>2922</v>
+        <v>2919</v>
       </c>
       <c r="F786" s="24" t="s">
-        <v>2922</v>
+        <v>2919</v>
       </c>
     </row>
     <row r="787" spans="1:6" ht="17.25" x14ac:dyDescent="0.35">
@@ -27405,7 +27420,7 @@
         <v>847</v>
       </c>
       <c r="B851" s="31" t="s">
-        <v>2844</v>
+        <v>2841</v>
       </c>
       <c r="C851" s="24" t="s">
         <v>2257</v>
@@ -27420,7 +27435,7 @@
         <v>2257</v>
       </c>
       <c r="H851" s="31" t="s">
-        <v>2890</v>
+        <v>2887</v>
       </c>
     </row>
     <row r="852" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
@@ -27443,7 +27458,7 @@
         <v>2260</v>
       </c>
       <c r="H852" s="31" t="s">
-        <v>2891</v>
+        <v>2888</v>
       </c>
     </row>
     <row r="853" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
@@ -27466,7 +27481,7 @@
         <v>2263</v>
       </c>
       <c r="H853" s="31" t="s">
-        <v>2892</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="854" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
@@ -27489,7 +27504,7 @@
         <v>2266</v>
       </c>
       <c r="H854" s="31" t="s">
-        <v>2893</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="855" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
@@ -27512,7 +27527,7 @@
         <v>2269</v>
       </c>
       <c r="H855" s="31" t="s">
-        <v>2894</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="856" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
@@ -27535,7 +27550,7 @@
         <v>2272</v>
       </c>
       <c r="H856" s="31" t="s">
-        <v>2895</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="857" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
@@ -27558,7 +27573,7 @@
         <v>2275</v>
       </c>
       <c r="H857" s="31" t="s">
-        <v>2896</v>
+        <v>2893</v>
       </c>
     </row>
     <row r="858" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
@@ -27581,7 +27596,7 @@
         <v>2278</v>
       </c>
       <c r="H858" s="31" t="s">
-        <v>2897</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="859" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
@@ -27604,7 +27619,7 @@
         <v>2281</v>
       </c>
       <c r="H859" s="31" t="s">
-        <v>2898</v>
+        <v>2895</v>
       </c>
     </row>
     <row r="860" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
@@ -27627,7 +27642,7 @@
         <v>2284</v>
       </c>
       <c r="H860" s="31" t="s">
-        <v>2899</v>
+        <v>2896</v>
       </c>
     </row>
     <row r="861" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
@@ -27650,7 +27665,7 @@
         <v>2287</v>
       </c>
       <c r="H861" s="31" t="s">
-        <v>2900</v>
+        <v>2897</v>
       </c>
     </row>
     <row r="862" spans="1:8" x14ac:dyDescent="0.35">
@@ -29892,7 +29907,7 @@
         <v>2613</v>
       </c>
       <c r="D974" s="1" t="s">
-        <v>2969</v>
+        <v>2966</v>
       </c>
       <c r="E974" s="1" t="s">
         <v>2613</v>
@@ -30029,7 +30044,7 @@
         <v>2632</v>
       </c>
       <c r="C981" s="27" t="s">
-        <v>2829</v>
+        <v>2827</v>
       </c>
       <c r="D981" s="27" t="s">
         <v>2634</v>
@@ -30049,7 +30064,7 @@
         <v>2635</v>
       </c>
       <c r="C982" s="27" t="s">
-        <v>2830</v>
+        <v>2828</v>
       </c>
       <c r="D982" s="27" t="s">
         <v>2637</v>
@@ -30069,7 +30084,7 @@
         <v>2638</v>
       </c>
       <c r="C983" s="28" t="s">
-        <v>2831</v>
+        <v>2829</v>
       </c>
       <c r="D983" s="28" t="s">
         <v>2640</v>
@@ -30129,7 +30144,7 @@
         <v>2647</v>
       </c>
       <c r="C986" s="27" t="s">
-        <v>2832</v>
+        <v>2830</v>
       </c>
       <c r="D986" s="27" t="s">
         <v>2649</v>
@@ -30149,7 +30164,7 @@
         <v>2650</v>
       </c>
       <c r="C987" s="27" t="s">
-        <v>2833</v>
+        <v>2831</v>
       </c>
       <c r="D987" s="27" t="s">
         <v>2652</v>
@@ -30229,7 +30244,7 @@
         <v>2662</v>
       </c>
       <c r="C991" s="1" t="s">
-        <v>2834</v>
+        <v>2832</v>
       </c>
       <c r="D991" s="1" t="s">
         <v>2664</v>
@@ -30249,10 +30264,10 @@
         <v>2665</v>
       </c>
       <c r="C992" s="23" t="s">
-        <v>2835</v>
+        <v>2833</v>
       </c>
       <c r="D992" s="23" t="s">
-        <v>2970</v>
+        <v>2967</v>
       </c>
       <c r="E992" s="23" t="s">
         <v>2666</v>
@@ -30269,7 +30284,7 @@
         <v>2667</v>
       </c>
       <c r="C993" s="1" t="s">
-        <v>2836</v>
+        <v>2834</v>
       </c>
       <c r="D993" s="1" t="s">
         <v>2669</v>
@@ -30289,16 +30304,16 @@
         <v>2670</v>
       </c>
       <c r="C994" s="29" t="s">
-        <v>2839</v>
+        <v>2836</v>
       </c>
       <c r="D994" s="23" t="s">
-        <v>2840</v>
+        <v>2837</v>
       </c>
       <c r="E994" s="29" t="s">
-        <v>2839</v>
+        <v>2836</v>
       </c>
       <c r="F994" s="29" t="s">
-        <v>2839</v>
+        <v>2836</v>
       </c>
     </row>
     <row r="995" spans="1:6" x14ac:dyDescent="0.35">
@@ -30909,16 +30924,16 @@
         <v>2761</v>
       </c>
       <c r="C1025" s="31" t="s">
-        <v>2842</v>
+        <v>2839</v>
       </c>
       <c r="D1025" s="1" t="s">
         <v>2762</v>
       </c>
       <c r="E1025" s="31" t="s">
-        <v>2842</v>
+        <v>2839</v>
       </c>
       <c r="F1025" s="31" t="s">
-        <v>2842</v>
+        <v>2839</v>
       </c>
     </row>
     <row r="1026" spans="1:6" x14ac:dyDescent="0.35">
@@ -30929,16 +30944,16 @@
         <v>2763</v>
       </c>
       <c r="C1026" s="31" t="s">
-        <v>2843</v>
+        <v>2840</v>
       </c>
       <c r="D1026" s="1" t="s">
         <v>2764</v>
       </c>
       <c r="E1026" s="31" t="s">
-        <v>2843</v>
+        <v>2840</v>
       </c>
       <c r="F1026" s="31" t="s">
-        <v>2843</v>
+        <v>2840</v>
       </c>
     </row>
     <row r="1027" spans="1:6" x14ac:dyDescent="0.35">
@@ -30949,16 +30964,16 @@
         <v>2765</v>
       </c>
       <c r="C1027" s="31" t="s">
-        <v>2841</v>
+        <v>2838</v>
       </c>
       <c r="D1027" s="1" t="s">
         <v>2766</v>
       </c>
       <c r="E1027" s="31" t="s">
-        <v>2841</v>
+        <v>2838</v>
       </c>
       <c r="F1027" s="31" t="s">
-        <v>2841</v>
+        <v>2838</v>
       </c>
     </row>
     <row r="1028" spans="1:6" x14ac:dyDescent="0.35">
@@ -31189,16 +31204,16 @@
         <v>2800</v>
       </c>
       <c r="C1040" s="31" t="s">
-        <v>2837</v>
+        <v>2969</v>
       </c>
       <c r="D1040" s="30" t="s">
-        <v>2802</v>
+        <v>2971</v>
       </c>
       <c r="E1040" s="31" t="s">
-        <v>2801</v>
+        <v>2969</v>
       </c>
       <c r="F1040" s="31" t="s">
-        <v>2801</v>
+        <v>2969</v>
       </c>
     </row>
     <row r="1041" spans="1:6" x14ac:dyDescent="0.35">
@@ -31206,19 +31221,19 @@
         <v>1036</v>
       </c>
       <c r="B1041" s="30" t="s">
-        <v>2803</v>
+        <v>2801</v>
       </c>
       <c r="C1041" s="31" t="s">
-        <v>2838</v>
+        <v>2835</v>
       </c>
       <c r="D1041" s="30" t="s">
-        <v>2804</v>
+        <v>2802</v>
       </c>
       <c r="E1041" s="31" t="s">
-        <v>2971</v>
+        <v>2968</v>
       </c>
       <c r="F1041" s="31" t="s">
-        <v>2971</v>
+        <v>2968</v>
       </c>
     </row>
     <row r="1042" spans="1:6" x14ac:dyDescent="0.35">
@@ -31226,19 +31241,19 @@
         <v>1037</v>
       </c>
       <c r="B1042" s="30" t="s">
+        <v>2803</v>
+      </c>
+      <c r="C1042" s="30" t="s">
+        <v>2970</v>
+      </c>
+      <c r="D1042" s="30" t="s">
         <v>2805</v>
       </c>
-      <c r="C1042" s="30" t="s">
-        <v>2806</v>
-      </c>
-      <c r="D1042" s="30" t="s">
-        <v>2807</v>
-      </c>
       <c r="E1042" s="30" t="s">
-        <v>2806</v>
+        <v>2804</v>
       </c>
       <c r="F1042" s="30" t="s">
-        <v>2806</v>
+        <v>2804</v>
       </c>
     </row>
     <row r="1043" spans="1:6" x14ac:dyDescent="0.35">
@@ -31246,19 +31261,19 @@
         <v>1038</v>
       </c>
       <c r="B1043" s="30" t="s">
+        <v>2806</v>
+      </c>
+      <c r="C1043" s="30" t="s">
+        <v>2807</v>
+      </c>
+      <c r="D1043" s="30" t="s">
         <v>2808</v>
       </c>
-      <c r="C1043" s="30" t="s">
-        <v>2809</v>
-      </c>
-      <c r="D1043" s="30" t="s">
-        <v>2810</v>
-      </c>
       <c r="E1043" s="30" t="s">
-        <v>2809</v>
+        <v>2807</v>
       </c>
       <c r="F1043" s="30" t="s">
-        <v>2809</v>
+        <v>2807</v>
       </c>
     </row>
     <row r="1044" spans="1:6" x14ac:dyDescent="0.35">
@@ -31266,19 +31281,19 @@
         <v>1039</v>
       </c>
       <c r="B1044" s="30" t="s">
+        <v>2809</v>
+      </c>
+      <c r="C1044" s="32" t="s">
+        <v>2810</v>
+      </c>
+      <c r="D1044" s="30" t="s">
         <v>2811</v>
       </c>
-      <c r="C1044" s="32" t="s">
-        <v>2812</v>
-      </c>
-      <c r="D1044" s="30" t="s">
-        <v>2813</v>
-      </c>
       <c r="E1044" s="32" t="s">
-        <v>2812</v>
+        <v>2810</v>
       </c>
       <c r="F1044" s="32" t="s">
-        <v>2812</v>
+        <v>2810</v>
       </c>
     </row>
     <row r="1045" spans="1:6" x14ac:dyDescent="0.35">
@@ -31286,13 +31301,13 @@
         <v>1040</v>
       </c>
       <c r="B1045" s="30" t="s">
-        <v>2814</v>
+        <v>2812</v>
       </c>
       <c r="C1045" s="30" t="s">
         <v>761</v>
       </c>
       <c r="D1045" s="30" t="s">
-        <v>2815</v>
+        <v>2813</v>
       </c>
       <c r="E1045" s="30" t="s">
         <v>761</v>
@@ -31306,19 +31321,39 @@
         <v>1041</v>
       </c>
       <c r="B1047" s="1" t="s">
+        <v>2814</v>
+      </c>
+      <c r="C1047" s="1" t="s">
+        <v>2815</v>
+      </c>
+      <c r="D1047" s="1" t="s">
         <v>2816</v>
       </c>
-      <c r="C1047" s="1" t="s">
-        <v>2817</v>
-      </c>
-      <c r="D1047" s="1" t="s">
-        <v>2818</v>
-      </c>
       <c r="E1047" s="1" t="s">
-        <v>2817</v>
+        <v>2815</v>
       </c>
       <c r="F1047" s="1" t="s">
-        <v>2817</v>
+        <v>2815</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1048" s="1">
+        <v>1042</v>
+      </c>
+      <c r="B1048" s="31" t="s">
+        <v>2974</v>
+      </c>
+      <c r="C1048" s="31" t="s">
+        <v>2973</v>
+      </c>
+      <c r="D1048" s="31" t="s">
+        <v>2972</v>
+      </c>
+      <c r="E1048" s="31" t="s">
+        <v>2973</v>
+      </c>
+      <c r="F1048" s="31" t="s">
+        <v>2973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat：fix area treasure and language
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/Language_多语言表.xlsx
+++ b/pet-simulator/Excel/Language_多语言表.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5314" uniqueCount="2996">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5314" uniqueCount="2997">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -7892,10 +7892,32 @@
     <t xml:space="preserve">Plaza_Text_12</t>
   </si>
   <si>
-    <t xml:space="preserve">{0} coins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{0}币</t>
+    <t xml:space="preserve">{0} rewards!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{0}币!</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{0} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">rewards!</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Plaza_Text_13</t>
@@ -9066,7 +9088,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
@@ -9157,6 +9179,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="0"/>
       <charset val="134"/>
     </font>
@@ -9409,7 +9438,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -9433,7 +9462,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -9688,8 +9717,8 @@
   </sheetPr>
   <dimension ref="A1:T1063"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1044" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1068" activeCellId="0" sqref="D1068"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A926" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H937" activeCellId="0" sqref="H937"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.12890625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29152,10 +29181,10 @@
         <v>2614</v>
       </c>
       <c r="E935" s="31" t="s">
-        <v>2613</v>
+        <v>2615</v>
       </c>
       <c r="F935" s="31" t="s">
-        <v>2613</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="936" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29163,19 +29192,19 @@
         <v>932</v>
       </c>
       <c r="B936" s="1" t="s">
-        <v>2615</v>
+        <v>2616</v>
       </c>
       <c r="C936" s="31" t="s">
-        <v>2616</v>
+        <v>2617</v>
       </c>
       <c r="D936" s="1" t="s">
+        <v>2618</v>
+      </c>
+      <c r="E936" s="31" t="s">
         <v>2617</v>
       </c>
-      <c r="E936" s="31" t="s">
-        <v>2616</v>
-      </c>
       <c r="F936" s="31" t="s">
-        <v>2616</v>
+        <v>2617</v>
       </c>
     </row>
     <row r="937" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29183,13 +29212,13 @@
         <v>933</v>
       </c>
       <c r="B937" s="1" t="s">
-        <v>2618</v>
+        <v>2619</v>
       </c>
       <c r="C937" s="31" t="s">
         <v>735</v>
       </c>
       <c r="D937" s="1" t="s">
-        <v>2619</v>
+        <v>2620</v>
       </c>
       <c r="E937" s="31" t="s">
         <v>735</v>
@@ -29203,19 +29232,19 @@
         <v>934</v>
       </c>
       <c r="B938" s="1" t="s">
-        <v>2620</v>
+        <v>2621</v>
       </c>
       <c r="C938" s="1" t="s">
-        <v>2621</v>
+        <v>2622</v>
       </c>
       <c r="D938" s="1" t="s">
+        <v>2623</v>
+      </c>
+      <c r="E938" s="1" t="s">
         <v>2622</v>
       </c>
-      <c r="E938" s="1" t="s">
-        <v>2621</v>
-      </c>
       <c r="F938" s="1" t="s">
-        <v>2621</v>
+        <v>2622</v>
       </c>
     </row>
     <row r="939" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29223,19 +29252,19 @@
         <v>935</v>
       </c>
       <c r="B939" s="1" t="s">
-        <v>2623</v>
+        <v>2624</v>
       </c>
       <c r="C939" s="1" t="s">
-        <v>2624</v>
+        <v>2625</v>
       </c>
       <c r="D939" s="1" t="s">
+        <v>2626</v>
+      </c>
+      <c r="E939" s="1" t="s">
         <v>2625</v>
       </c>
-      <c r="E939" s="1" t="s">
-        <v>2624</v>
-      </c>
       <c r="F939" s="1" t="s">
-        <v>2624</v>
+        <v>2625</v>
       </c>
     </row>
     <row r="940" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29243,19 +29272,19 @@
         <v>936</v>
       </c>
       <c r="B940" s="1" t="s">
-        <v>2626</v>
+        <v>2627</v>
       </c>
       <c r="C940" s="1" t="s">
-        <v>2627</v>
+        <v>2628</v>
       </c>
       <c r="D940" s="1" t="s">
+        <v>2629</v>
+      </c>
+      <c r="E940" s="1" t="s">
         <v>2628</v>
       </c>
-      <c r="E940" s="1" t="s">
-        <v>2627</v>
-      </c>
       <c r="F940" s="1" t="s">
-        <v>2627</v>
+        <v>2628</v>
       </c>
     </row>
     <row r="941" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29263,19 +29292,19 @@
         <v>937</v>
       </c>
       <c r="B941" s="1" t="s">
-        <v>2629</v>
+        <v>2630</v>
       </c>
       <c r="C941" s="1" t="s">
-        <v>2630</v>
+        <v>2631</v>
       </c>
       <c r="D941" s="1" t="s">
+        <v>2632</v>
+      </c>
+      <c r="E941" s="1" t="s">
         <v>2631</v>
       </c>
-      <c r="E941" s="1" t="s">
-        <v>2630</v>
-      </c>
       <c r="F941" s="1" t="s">
-        <v>2630</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="942" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29283,19 +29312,19 @@
         <v>938</v>
       </c>
       <c r="B942" s="1" t="s">
-        <v>2632</v>
+        <v>2633</v>
       </c>
       <c r="C942" s="1" t="s">
-        <v>2633</v>
+        <v>2634</v>
       </c>
       <c r="D942" s="1" t="s">
+        <v>2635</v>
+      </c>
+      <c r="E942" s="1" t="s">
         <v>2634</v>
       </c>
-      <c r="E942" s="1" t="s">
-        <v>2633</v>
-      </c>
       <c r="F942" s="1" t="s">
-        <v>2633</v>
+        <v>2634</v>
       </c>
     </row>
     <row r="943" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29303,19 +29332,19 @@
         <v>939</v>
       </c>
       <c r="B943" s="1" t="s">
-        <v>2635</v>
+        <v>2636</v>
       </c>
       <c r="C943" s="1" t="s">
-        <v>2636</v>
+        <v>2637</v>
       </c>
       <c r="D943" s="1" t="s">
+        <v>2638</v>
+      </c>
+      <c r="E943" s="1" t="s">
         <v>2637</v>
       </c>
-      <c r="E943" s="1" t="s">
-        <v>2636</v>
-      </c>
       <c r="F943" s="1" t="s">
-        <v>2636</v>
+        <v>2637</v>
       </c>
     </row>
     <row r="944" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29323,19 +29352,19 @@
         <v>940</v>
       </c>
       <c r="B944" s="1" t="s">
-        <v>2638</v>
+        <v>2639</v>
       </c>
       <c r="C944" s="1" t="s">
-        <v>2639</v>
+        <v>2640</v>
       </c>
       <c r="D944" s="1" t="s">
+        <v>2641</v>
+      </c>
+      <c r="E944" s="1" t="s">
         <v>2640</v>
       </c>
-      <c r="E944" s="1" t="s">
-        <v>2639</v>
-      </c>
       <c r="F944" s="1" t="s">
-        <v>2639</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="945" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29343,19 +29372,19 @@
         <v>941</v>
       </c>
       <c r="B945" s="1" t="s">
-        <v>2641</v>
+        <v>2642</v>
       </c>
       <c r="C945" s="1" t="s">
-        <v>2642</v>
+        <v>2643</v>
       </c>
       <c r="D945" s="1" t="s">
+        <v>2644</v>
+      </c>
+      <c r="E945" s="1" t="s">
         <v>2643</v>
       </c>
-      <c r="E945" s="1" t="s">
-        <v>2642</v>
-      </c>
       <c r="F945" s="1" t="s">
-        <v>2642</v>
+        <v>2643</v>
       </c>
     </row>
     <row r="946" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29363,19 +29392,19 @@
         <v>942</v>
       </c>
       <c r="B946" s="1" t="s">
-        <v>2644</v>
+        <v>2645</v>
       </c>
       <c r="C946" s="1" t="s">
-        <v>2645</v>
+        <v>2646</v>
       </c>
       <c r="D946" s="1" t="s">
+        <v>2647</v>
+      </c>
+      <c r="E946" s="1" t="s">
         <v>2646</v>
       </c>
-      <c r="E946" s="1" t="s">
-        <v>2645</v>
-      </c>
       <c r="F946" s="1" t="s">
-        <v>2645</v>
+        <v>2646</v>
       </c>
     </row>
     <row r="947" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29383,19 +29412,19 @@
         <v>943</v>
       </c>
       <c r="B947" s="1" t="s">
-        <v>2647</v>
+        <v>2648</v>
       </c>
       <c r="C947" s="1" t="s">
-        <v>2648</v>
+        <v>2649</v>
       </c>
       <c r="D947" s="1" t="s">
+        <v>2650</v>
+      </c>
+      <c r="E947" s="1" t="s">
         <v>2649</v>
       </c>
-      <c r="E947" s="1" t="s">
-        <v>2648</v>
-      </c>
       <c r="F947" s="1" t="s">
-        <v>2648</v>
+        <v>2649</v>
       </c>
     </row>
     <row r="948" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29403,19 +29432,19 @@
         <v>944</v>
       </c>
       <c r="B948" s="1" t="s">
-        <v>2650</v>
+        <v>2651</v>
       </c>
       <c r="C948" s="1" t="s">
-        <v>2651</v>
+        <v>2652</v>
       </c>
       <c r="D948" s="1" t="s">
         <v>2582</v>
       </c>
       <c r="E948" s="1" t="s">
-        <v>2651</v>
+        <v>2652</v>
       </c>
       <c r="F948" s="1" t="s">
-        <v>2651</v>
+        <v>2652</v>
       </c>
     </row>
     <row r="949" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29423,19 +29452,19 @@
         <v>945</v>
       </c>
       <c r="B949" s="1" t="s">
-        <v>2652</v>
+        <v>2653</v>
       </c>
       <c r="C949" s="1" t="s">
-        <v>2653</v>
+        <v>2654</v>
       </c>
       <c r="D949" s="1" t="s">
+        <v>2655</v>
+      </c>
+      <c r="E949" s="1" t="s">
         <v>2654</v>
       </c>
-      <c r="E949" s="1" t="s">
-        <v>2653</v>
-      </c>
       <c r="F949" s="1" t="s">
-        <v>2653</v>
+        <v>2654</v>
       </c>
     </row>
     <row r="950" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29443,19 +29472,19 @@
         <v>946</v>
       </c>
       <c r="B950" s="1" t="s">
-        <v>2655</v>
+        <v>2656</v>
       </c>
       <c r="C950" s="1" t="s">
-        <v>2656</v>
+        <v>2657</v>
       </c>
       <c r="D950" s="1" t="s">
+        <v>2658</v>
+      </c>
+      <c r="E950" s="1" t="s">
         <v>2657</v>
       </c>
-      <c r="E950" s="1" t="s">
-        <v>2656</v>
-      </c>
       <c r="F950" s="1" t="s">
-        <v>2656</v>
+        <v>2657</v>
       </c>
     </row>
     <row r="951" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29463,19 +29492,19 @@
         <v>947</v>
       </c>
       <c r="B951" s="1" t="s">
-        <v>2658</v>
+        <v>2659</v>
       </c>
       <c r="C951" s="1" t="s">
-        <v>2659</v>
+        <v>2660</v>
       </c>
       <c r="D951" s="1" t="s">
+        <v>2661</v>
+      </c>
+      <c r="E951" s="1" t="s">
         <v>2660</v>
       </c>
-      <c r="E951" s="1" t="s">
-        <v>2659</v>
-      </c>
       <c r="F951" s="1" t="s">
-        <v>2659</v>
+        <v>2660</v>
       </c>
     </row>
     <row r="952" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29483,19 +29512,19 @@
         <v>948</v>
       </c>
       <c r="B952" s="1" t="s">
-        <v>2661</v>
+        <v>2662</v>
       </c>
       <c r="C952" s="1" t="s">
-        <v>2662</v>
+        <v>2663</v>
       </c>
       <c r="D952" s="1" t="s">
+        <v>2664</v>
+      </c>
+      <c r="E952" s="1" t="s">
         <v>2663</v>
       </c>
-      <c r="E952" s="1" t="s">
-        <v>2662</v>
-      </c>
       <c r="F952" s="1" t="s">
-        <v>2662</v>
+        <v>2663</v>
       </c>
     </row>
     <row r="953" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29503,19 +29532,19 @@
         <v>949</v>
       </c>
       <c r="B953" s="1" t="s">
-        <v>2664</v>
+        <v>2665</v>
       </c>
       <c r="C953" s="1" t="s">
-        <v>2665</v>
+        <v>2666</v>
       </c>
       <c r="D953" s="1" t="s">
+        <v>2667</v>
+      </c>
+      <c r="E953" s="1" t="s">
         <v>2666</v>
       </c>
-      <c r="E953" s="1" t="s">
-        <v>2665</v>
-      </c>
       <c r="F953" s="1" t="s">
-        <v>2665</v>
+        <v>2666</v>
       </c>
     </row>
     <row r="954" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29523,19 +29552,19 @@
         <v>950</v>
       </c>
       <c r="B954" s="1" t="s">
-        <v>2667</v>
+        <v>2668</v>
       </c>
       <c r="C954" s="1" t="s">
-        <v>2668</v>
+        <v>2669</v>
       </c>
       <c r="D954" s="1" t="s">
+        <v>2670</v>
+      </c>
+      <c r="E954" s="1" t="s">
         <v>2669</v>
       </c>
-      <c r="E954" s="1" t="s">
-        <v>2668</v>
-      </c>
       <c r="F954" s="1" t="s">
-        <v>2668</v>
+        <v>2669</v>
       </c>
     </row>
     <row r="955" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29543,19 +29572,19 @@
         <v>951</v>
       </c>
       <c r="B955" s="1" t="s">
-        <v>2670</v>
+        <v>2671</v>
       </c>
       <c r="C955" s="1" t="s">
-        <v>2671</v>
+        <v>2672</v>
       </c>
       <c r="D955" s="1" t="s">
+        <v>2673</v>
+      </c>
+      <c r="E955" s="1" t="s">
         <v>2672</v>
       </c>
-      <c r="E955" s="1" t="s">
-        <v>2671</v>
-      </c>
       <c r="F955" s="1" t="s">
-        <v>2671</v>
+        <v>2672</v>
       </c>
     </row>
     <row r="956" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29563,19 +29592,19 @@
         <v>952</v>
       </c>
       <c r="B956" s="1" t="s">
-        <v>2673</v>
+        <v>2674</v>
       </c>
       <c r="C956" s="1" t="s">
-        <v>2674</v>
+        <v>2675</v>
       </c>
       <c r="D956" s="1" t="s">
+        <v>2676</v>
+      </c>
+      <c r="E956" s="1" t="s">
         <v>2675</v>
       </c>
-      <c r="E956" s="1" t="s">
-        <v>2674</v>
-      </c>
       <c r="F956" s="1" t="s">
-        <v>2674</v>
+        <v>2675</v>
       </c>
     </row>
     <row r="957" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29583,19 +29612,19 @@
         <v>953</v>
       </c>
       <c r="B957" s="1" t="s">
-        <v>2676</v>
+        <v>2677</v>
       </c>
       <c r="C957" s="1" t="s">
-        <v>2677</v>
+        <v>2678</v>
       </c>
       <c r="D957" s="1" t="s">
+        <v>2679</v>
+      </c>
+      <c r="E957" s="1" t="s">
         <v>2678</v>
       </c>
-      <c r="E957" s="1" t="s">
-        <v>2677</v>
-      </c>
       <c r="F957" s="1" t="s">
-        <v>2677</v>
+        <v>2678</v>
       </c>
     </row>
     <row r="958" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29603,19 +29632,19 @@
         <v>954</v>
       </c>
       <c r="B958" s="1" t="s">
-        <v>2679</v>
+        <v>2680</v>
       </c>
       <c r="C958" s="1" t="s">
-        <v>2680</v>
+        <v>2681</v>
       </c>
       <c r="D958" s="1" t="s">
+        <v>2682</v>
+      </c>
+      <c r="E958" s="1" t="s">
         <v>2681</v>
       </c>
-      <c r="E958" s="1" t="s">
-        <v>2680</v>
-      </c>
       <c r="F958" s="1" t="s">
-        <v>2680</v>
+        <v>2681</v>
       </c>
     </row>
     <row r="959" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29623,19 +29652,19 @@
         <v>955</v>
       </c>
       <c r="B959" s="1" t="s">
-        <v>2682</v>
+        <v>2683</v>
       </c>
       <c r="C959" s="1" t="s">
-        <v>2683</v>
+        <v>2684</v>
       </c>
       <c r="D959" s="1" t="s">
+        <v>2685</v>
+      </c>
+      <c r="E959" s="1" t="s">
         <v>2684</v>
       </c>
-      <c r="E959" s="1" t="s">
-        <v>2683</v>
-      </c>
       <c r="F959" s="1" t="s">
-        <v>2683</v>
+        <v>2684</v>
       </c>
     </row>
     <row r="960" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29643,19 +29672,19 @@
         <v>956</v>
       </c>
       <c r="B960" s="1" t="s">
-        <v>2685</v>
+        <v>2686</v>
       </c>
       <c r="C960" s="1" t="s">
-        <v>2686</v>
+        <v>2687</v>
       </c>
       <c r="D960" s="1" t="s">
+        <v>2688</v>
+      </c>
+      <c r="E960" s="1" t="s">
         <v>2687</v>
       </c>
-      <c r="E960" s="1" t="s">
-        <v>2686</v>
-      </c>
       <c r="F960" s="1" t="s">
-        <v>2686</v>
+        <v>2687</v>
       </c>
     </row>
     <row r="961" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29663,19 +29692,19 @@
         <v>957</v>
       </c>
       <c r="B961" s="1" t="s">
-        <v>2688</v>
+        <v>2689</v>
       </c>
       <c r="C961" s="1" t="s">
-        <v>2689</v>
+        <v>2690</v>
       </c>
       <c r="D961" s="1" t="s">
+        <v>2691</v>
+      </c>
+      <c r="E961" s="1" t="s">
         <v>2690</v>
       </c>
-      <c r="E961" s="1" t="s">
-        <v>2689</v>
-      </c>
       <c r="F961" s="1" t="s">
-        <v>2689</v>
+        <v>2690</v>
       </c>
     </row>
     <row r="962" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29683,19 +29712,19 @@
         <v>958</v>
       </c>
       <c r="B962" s="1" t="s">
-        <v>2691</v>
+        <v>2692</v>
       </c>
       <c r="C962" s="1" t="s">
-        <v>2692</v>
+        <v>2693</v>
       </c>
       <c r="D962" s="1" t="s">
+        <v>2694</v>
+      </c>
+      <c r="E962" s="1" t="s">
         <v>2693</v>
       </c>
-      <c r="E962" s="1" t="s">
-        <v>2692</v>
-      </c>
       <c r="F962" s="1" t="s">
-        <v>2692</v>
+        <v>2693</v>
       </c>
     </row>
     <row r="963" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29703,19 +29732,19 @@
         <v>959</v>
       </c>
       <c r="B963" s="1" t="s">
-        <v>2694</v>
+        <v>2695</v>
       </c>
       <c r="C963" s="1" t="s">
-        <v>2695</v>
+        <v>2696</v>
       </c>
       <c r="D963" s="1" t="s">
+        <v>2697</v>
+      </c>
+      <c r="E963" s="1" t="s">
         <v>2696</v>
       </c>
-      <c r="E963" s="1" t="s">
-        <v>2695</v>
-      </c>
       <c r="F963" s="1" t="s">
-        <v>2695</v>
+        <v>2696</v>
       </c>
     </row>
     <row r="964" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29723,19 +29752,19 @@
         <v>960</v>
       </c>
       <c r="B964" s="1" t="s">
-        <v>2697</v>
+        <v>2698</v>
       </c>
       <c r="C964" s="1" t="s">
-        <v>2698</v>
+        <v>2699</v>
       </c>
       <c r="D964" s="1" t="s">
+        <v>2700</v>
+      </c>
+      <c r="E964" s="1" t="s">
         <v>2699</v>
       </c>
-      <c r="E964" s="1" t="s">
-        <v>2698</v>
-      </c>
       <c r="F964" s="1" t="s">
-        <v>2698</v>
+        <v>2699</v>
       </c>
     </row>
     <row r="965" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29743,19 +29772,19 @@
         <v>961</v>
       </c>
       <c r="B965" s="1" t="s">
-        <v>2700</v>
+        <v>2701</v>
       </c>
       <c r="C965" s="1" t="s">
-        <v>2701</v>
+        <v>2702</v>
       </c>
       <c r="D965" s="1" t="s">
+        <v>2703</v>
+      </c>
+      <c r="E965" s="1" t="s">
         <v>2702</v>
       </c>
-      <c r="E965" s="1" t="s">
-        <v>2701</v>
-      </c>
       <c r="F965" s="1" t="s">
-        <v>2701</v>
+        <v>2702</v>
       </c>
     </row>
     <row r="966" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29763,19 +29792,19 @@
         <v>962</v>
       </c>
       <c r="B966" s="1" t="s">
-        <v>2703</v>
+        <v>2704</v>
       </c>
       <c r="C966" s="1" t="s">
-        <v>2704</v>
+        <v>2705</v>
       </c>
       <c r="D966" s="1" t="s">
+        <v>2706</v>
+      </c>
+      <c r="E966" s="1" t="s">
         <v>2705</v>
       </c>
-      <c r="E966" s="1" t="s">
-        <v>2704</v>
-      </c>
       <c r="F966" s="1" t="s">
-        <v>2704</v>
+        <v>2705</v>
       </c>
     </row>
     <row r="967" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29783,19 +29812,19 @@
         <v>963</v>
       </c>
       <c r="B967" s="1" t="s">
-        <v>2706</v>
+        <v>2707</v>
       </c>
       <c r="C967" s="1" t="s">
-        <v>2707</v>
+        <v>2708</v>
       </c>
       <c r="D967" s="1" t="s">
+        <v>2709</v>
+      </c>
+      <c r="E967" s="1" t="s">
         <v>2708</v>
       </c>
-      <c r="E967" s="1" t="s">
-        <v>2707</v>
-      </c>
       <c r="F967" s="1" t="s">
-        <v>2707</v>
+        <v>2708</v>
       </c>
     </row>
     <row r="968" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29803,19 +29832,19 @@
         <v>964</v>
       </c>
       <c r="B968" s="1" t="s">
-        <v>2709</v>
+        <v>2710</v>
       </c>
       <c r="C968" s="36" t="s">
-        <v>2710</v>
+        <v>2711</v>
       </c>
       <c r="D968" s="1" t="s">
+        <v>2712</v>
+      </c>
+      <c r="E968" s="36" t="s">
         <v>2711</v>
       </c>
-      <c r="E968" s="36" t="s">
-        <v>2710</v>
-      </c>
       <c r="F968" s="36" t="s">
-        <v>2710</v>
+        <v>2711</v>
       </c>
     </row>
     <row r="969" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29823,19 +29852,19 @@
         <v>965</v>
       </c>
       <c r="B969" s="1" t="s">
-        <v>2712</v>
+        <v>2713</v>
       </c>
       <c r="C969" s="1" t="s">
-        <v>2713</v>
+        <v>2714</v>
       </c>
       <c r="D969" s="1" t="s">
+        <v>2715</v>
+      </c>
+      <c r="E969" s="1" t="s">
         <v>2714</v>
       </c>
-      <c r="E969" s="1" t="s">
-        <v>2713</v>
-      </c>
       <c r="F969" s="1" t="s">
-        <v>2713</v>
+        <v>2714</v>
       </c>
     </row>
     <row r="970" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29843,19 +29872,19 @@
         <v>966</v>
       </c>
       <c r="B970" s="1" t="s">
-        <v>2715</v>
+        <v>2716</v>
       </c>
       <c r="C970" s="36" t="s">
-        <v>2716</v>
+        <v>2717</v>
       </c>
       <c r="D970" s="1" t="s">
+        <v>2718</v>
+      </c>
+      <c r="E970" s="36" t="s">
         <v>2717</v>
       </c>
-      <c r="E970" s="36" t="s">
-        <v>2716</v>
-      </c>
       <c r="F970" s="36" t="s">
-        <v>2716</v>
+        <v>2717</v>
       </c>
     </row>
     <row r="971" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29863,19 +29892,19 @@
         <v>967</v>
       </c>
       <c r="B971" s="1" t="s">
-        <v>2718</v>
+        <v>2719</v>
       </c>
       <c r="C971" s="1" t="s">
-        <v>2719</v>
+        <v>2720</v>
       </c>
       <c r="D971" s="1" t="s">
+        <v>2721</v>
+      </c>
+      <c r="E971" s="1" t="s">
         <v>2720</v>
       </c>
-      <c r="E971" s="1" t="s">
-        <v>2719</v>
-      </c>
       <c r="F971" s="1" t="s">
-        <v>2719</v>
+        <v>2720</v>
       </c>
     </row>
     <row r="972" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29883,19 +29912,19 @@
         <v>968</v>
       </c>
       <c r="B972" s="1" t="s">
-        <v>2721</v>
+        <v>2722</v>
       </c>
       <c r="C972" s="36" t="s">
-        <v>2722</v>
+        <v>2723</v>
       </c>
       <c r="D972" s="1" t="s">
+        <v>2724</v>
+      </c>
+      <c r="E972" s="36" t="s">
         <v>2723</v>
       </c>
-      <c r="E972" s="36" t="s">
-        <v>2722</v>
-      </c>
       <c r="F972" s="36" t="s">
-        <v>2722</v>
+        <v>2723</v>
       </c>
     </row>
     <row r="973" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29903,13 +29932,13 @@
         <v>969</v>
       </c>
       <c r="B973" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C973" s="1" t="s">
         <v>1939</v>
       </c>
       <c r="D973" s="1" t="s">
-        <v>2725</v>
+        <v>2726</v>
       </c>
       <c r="E973" s="1" t="s">
         <v>1939</v>
@@ -29923,19 +29952,19 @@
         <v>970</v>
       </c>
       <c r="B974" s="1" t="s">
-        <v>2726</v>
+        <v>2727</v>
       </c>
       <c r="C974" s="1" t="s">
-        <v>2727</v>
+        <v>2728</v>
       </c>
       <c r="D974" s="1" t="s">
+        <v>2729</v>
+      </c>
+      <c r="E974" s="1" t="s">
         <v>2728</v>
       </c>
-      <c r="E974" s="1" t="s">
-        <v>2727</v>
-      </c>
       <c r="F974" s="1" t="s">
-        <v>2727</v>
+        <v>2728</v>
       </c>
     </row>
     <row r="975" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29943,19 +29972,19 @@
         <v>971</v>
       </c>
       <c r="B975" s="1" t="s">
-        <v>2729</v>
+        <v>2730</v>
       </c>
       <c r="C975" s="1" t="s">
-        <v>2730</v>
+        <v>2731</v>
       </c>
       <c r="D975" s="1" t="s">
+        <v>2732</v>
+      </c>
+      <c r="E975" s="1" t="s">
         <v>2731</v>
       </c>
-      <c r="E975" s="1" t="s">
-        <v>2730</v>
-      </c>
       <c r="F975" s="1" t="s">
-        <v>2730</v>
+        <v>2731</v>
       </c>
     </row>
     <row r="976" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29963,19 +29992,19 @@
         <v>972</v>
       </c>
       <c r="B976" s="1" t="s">
-        <v>2732</v>
+        <v>2733</v>
       </c>
       <c r="C976" s="1" t="s">
-        <v>2733</v>
+        <v>2734</v>
       </c>
       <c r="D976" s="1" t="s">
+        <v>2735</v>
+      </c>
+      <c r="E976" s="1" t="s">
         <v>2734</v>
       </c>
-      <c r="E976" s="1" t="s">
-        <v>2733</v>
-      </c>
       <c r="F976" s="1" t="s">
-        <v>2733</v>
+        <v>2734</v>
       </c>
     </row>
     <row r="977" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29983,19 +30012,19 @@
         <v>973</v>
       </c>
       <c r="B977" s="1" t="s">
-        <v>2735</v>
+        <v>2736</v>
       </c>
       <c r="C977" s="1" t="s">
-        <v>2736</v>
+        <v>2737</v>
       </c>
       <c r="D977" s="1" t="s">
+        <v>2738</v>
+      </c>
+      <c r="E977" s="1" t="s">
         <v>2737</v>
       </c>
-      <c r="E977" s="1" t="s">
-        <v>2736</v>
-      </c>
       <c r="F977" s="1" t="s">
-        <v>2736</v>
+        <v>2737</v>
       </c>
     </row>
     <row r="978" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30003,19 +30032,19 @@
         <v>974</v>
       </c>
       <c r="B978" s="1" t="s">
-        <v>2738</v>
+        <v>2739</v>
       </c>
       <c r="C978" s="1" t="s">
-        <v>2739</v>
+        <v>2740</v>
       </c>
       <c r="D978" s="1" t="s">
+        <v>2741</v>
+      </c>
+      <c r="E978" s="1" t="s">
         <v>2740</v>
       </c>
-      <c r="E978" s="1" t="s">
-        <v>2739</v>
-      </c>
       <c r="F978" s="1" t="s">
-        <v>2739</v>
+        <v>2740</v>
       </c>
     </row>
     <row r="979" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30023,19 +30052,19 @@
         <v>975</v>
       </c>
       <c r="B979" s="1" t="s">
-        <v>2741</v>
+        <v>2742</v>
       </c>
       <c r="C979" s="1" t="s">
-        <v>2742</v>
+        <v>2743</v>
       </c>
       <c r="D979" s="1" t="s">
+        <v>2744</v>
+      </c>
+      <c r="E979" s="1" t="s">
         <v>2743</v>
       </c>
-      <c r="E979" s="1" t="s">
-        <v>2742</v>
-      </c>
       <c r="F979" s="1" t="s">
-        <v>2742</v>
+        <v>2743</v>
       </c>
     </row>
     <row r="980" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30043,19 +30072,19 @@
         <v>976</v>
       </c>
       <c r="B980" s="1" t="s">
-        <v>2744</v>
+        <v>2745</v>
       </c>
       <c r="C980" s="1" t="s">
-        <v>2745</v>
+        <v>2746</v>
       </c>
       <c r="D980" s="1" t="s">
+        <v>2747</v>
+      </c>
+      <c r="E980" s="1" t="s">
         <v>2746</v>
       </c>
-      <c r="E980" s="1" t="s">
-        <v>2745</v>
-      </c>
       <c r="F980" s="1" t="s">
-        <v>2745</v>
+        <v>2746</v>
       </c>
     </row>
     <row r="981" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30063,19 +30092,19 @@
         <v>977</v>
       </c>
       <c r="B981" s="1" t="s">
-        <v>2747</v>
+        <v>2748</v>
       </c>
       <c r="C981" s="37" t="s">
-        <v>2748</v>
+        <v>2749</v>
       </c>
       <c r="D981" s="37" t="s">
-        <v>2749</v>
+        <v>2750</v>
       </c>
       <c r="E981" s="37" t="s">
-        <v>2750</v>
+        <v>2751</v>
       </c>
       <c r="F981" s="37" t="s">
-        <v>2750</v>
+        <v>2751</v>
       </c>
     </row>
     <row r="982" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30083,19 +30112,19 @@
         <v>978</v>
       </c>
       <c r="B982" s="1" t="s">
-        <v>2751</v>
+        <v>2752</v>
       </c>
       <c r="C982" s="37" t="s">
-        <v>2752</v>
+        <v>2753</v>
       </c>
       <c r="D982" s="37" t="s">
-        <v>2753</v>
+        <v>2754</v>
       </c>
       <c r="E982" s="37" t="s">
-        <v>2754</v>
+        <v>2755</v>
       </c>
       <c r="F982" s="37" t="s">
-        <v>2754</v>
+        <v>2755</v>
       </c>
     </row>
     <row r="983" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30103,19 +30132,19 @@
         <v>979</v>
       </c>
       <c r="B983" s="1" t="s">
-        <v>2755</v>
+        <v>2756</v>
       </c>
       <c r="C983" s="38" t="s">
-        <v>2756</v>
+        <v>2757</v>
       </c>
       <c r="D983" s="38" t="s">
-        <v>2757</v>
+        <v>2758</v>
       </c>
       <c r="E983" s="38" t="s">
-        <v>2758</v>
+        <v>2759</v>
       </c>
       <c r="F983" s="38" t="s">
-        <v>2758</v>
+        <v>2759</v>
       </c>
     </row>
     <row r="984" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30123,19 +30152,19 @@
         <v>980</v>
       </c>
       <c r="B984" s="1" t="s">
-        <v>2759</v>
+        <v>2760</v>
       </c>
       <c r="C984" s="38" t="s">
-        <v>2760</v>
+        <v>2761</v>
       </c>
       <c r="D984" s="38" t="s">
+        <v>2762</v>
+      </c>
+      <c r="E984" s="38" t="s">
         <v>2761</v>
       </c>
-      <c r="E984" s="38" t="s">
-        <v>2760</v>
-      </c>
       <c r="F984" s="38" t="s">
-        <v>2760</v>
+        <v>2761</v>
       </c>
     </row>
     <row r="985" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30143,19 +30172,19 @@
         <v>981</v>
       </c>
       <c r="B985" s="1" t="s">
-        <v>2762</v>
+        <v>2763</v>
       </c>
       <c r="C985" s="38" t="s">
-        <v>2763</v>
+        <v>2764</v>
       </c>
       <c r="D985" s="38" t="s">
+        <v>2765</v>
+      </c>
+      <c r="E985" s="38" t="s">
         <v>2764</v>
       </c>
-      <c r="E985" s="38" t="s">
-        <v>2763</v>
-      </c>
       <c r="F985" s="38" t="s">
-        <v>2763</v>
+        <v>2764</v>
       </c>
     </row>
     <row r="986" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30163,19 +30192,19 @@
         <v>982</v>
       </c>
       <c r="B986" s="1" t="s">
-        <v>2765</v>
+        <v>2766</v>
       </c>
       <c r="C986" s="37" t="s">
-        <v>2766</v>
+        <v>2767</v>
       </c>
       <c r="D986" s="37" t="s">
-        <v>2767</v>
+        <v>2768</v>
       </c>
       <c r="E986" s="37" t="s">
-        <v>2768</v>
+        <v>2769</v>
       </c>
       <c r="F986" s="37" t="s">
-        <v>2768</v>
+        <v>2769</v>
       </c>
     </row>
     <row r="987" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30183,19 +30212,19 @@
         <v>983</v>
       </c>
       <c r="B987" s="1" t="s">
-        <v>2769</v>
+        <v>2770</v>
       </c>
       <c r="C987" s="37" t="s">
-        <v>2770</v>
+        <v>2771</v>
       </c>
       <c r="D987" s="37" t="s">
-        <v>2771</v>
+        <v>2772</v>
       </c>
       <c r="E987" s="37" t="s">
-        <v>2772</v>
+        <v>2773</v>
       </c>
       <c r="F987" s="37" t="s">
-        <v>2772</v>
+        <v>2773</v>
       </c>
     </row>
     <row r="988" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30203,19 +30232,19 @@
         <v>984</v>
       </c>
       <c r="B988" s="1" t="s">
-        <v>2773</v>
+        <v>2774</v>
       </c>
       <c r="C988" s="38" t="s">
-        <v>2774</v>
+        <v>2775</v>
       </c>
       <c r="D988" s="38" t="s">
+        <v>2776</v>
+      </c>
+      <c r="E988" s="38" t="s">
         <v>2775</v>
       </c>
-      <c r="E988" s="38" t="s">
-        <v>2774</v>
-      </c>
       <c r="F988" s="38" t="s">
-        <v>2774</v>
+        <v>2775</v>
       </c>
     </row>
     <row r="989" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30223,19 +30252,19 @@
         <v>985</v>
       </c>
       <c r="B989" s="1" t="s">
-        <v>2776</v>
+        <v>2777</v>
       </c>
       <c r="C989" s="38" t="s">
-        <v>2777</v>
+        <v>2778</v>
       </c>
       <c r="D989" s="38" t="s">
+        <v>2779</v>
+      </c>
+      <c r="E989" s="38" t="s">
         <v>2778</v>
       </c>
-      <c r="E989" s="38" t="s">
-        <v>2777</v>
-      </c>
       <c r="F989" s="38" t="s">
-        <v>2777</v>
+        <v>2778</v>
       </c>
     </row>
     <row r="990" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30243,19 +30272,19 @@
         <v>986</v>
       </c>
       <c r="B990" s="1" t="s">
-        <v>2779</v>
+        <v>2780</v>
       </c>
       <c r="C990" s="38" t="s">
-        <v>2780</v>
+        <v>2781</v>
       </c>
       <c r="D990" s="38" t="s">
+        <v>2782</v>
+      </c>
+      <c r="E990" s="38" t="s">
         <v>2781</v>
       </c>
-      <c r="E990" s="38" t="s">
-        <v>2780</v>
-      </c>
       <c r="F990" s="38" t="s">
-        <v>2780</v>
+        <v>2781</v>
       </c>
     </row>
     <row r="991" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30263,19 +30292,19 @@
         <v>987</v>
       </c>
       <c r="B991" s="1" t="s">
-        <v>2782</v>
+        <v>2783</v>
       </c>
       <c r="C991" s="1" t="s">
-        <v>2783</v>
+        <v>2784</v>
       </c>
       <c r="D991" s="1" t="s">
-        <v>2784</v>
+        <v>2785</v>
       </c>
       <c r="E991" s="1" t="s">
-        <v>2785</v>
+        <v>2786</v>
       </c>
       <c r="F991" s="1" t="s">
-        <v>2785</v>
+        <v>2786</v>
       </c>
     </row>
     <row r="992" customFormat="false" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30283,19 +30312,19 @@
         <v>988</v>
       </c>
       <c r="B992" s="1" t="s">
-        <v>2786</v>
+        <v>2787</v>
       </c>
       <c r="C992" s="30" t="s">
-        <v>2787</v>
+        <v>2788</v>
       </c>
       <c r="D992" s="30" t="s">
-        <v>2788</v>
+        <v>2789</v>
       </c>
       <c r="E992" s="30" t="s">
-        <v>2789</v>
+        <v>2790</v>
       </c>
       <c r="F992" s="30" t="s">
-        <v>2789</v>
+        <v>2790</v>
       </c>
     </row>
     <row r="993" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30303,19 +30332,19 @@
         <v>989</v>
       </c>
       <c r="B993" s="1" t="s">
-        <v>2790</v>
+        <v>2791</v>
       </c>
       <c r="C993" s="1" t="s">
-        <v>2791</v>
+        <v>2792</v>
       </c>
       <c r="D993" s="1" t="s">
-        <v>2792</v>
+        <v>2793</v>
       </c>
       <c r="E993" s="1" t="s">
-        <v>2793</v>
+        <v>2794</v>
       </c>
       <c r="F993" s="1" t="s">
-        <v>2793</v>
+        <v>2794</v>
       </c>
     </row>
     <row r="994" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30323,19 +30352,19 @@
         <v>990</v>
       </c>
       <c r="B994" s="1" t="s">
-        <v>2794</v>
+        <v>2795</v>
       </c>
       <c r="C994" s="39" t="s">
-        <v>2795</v>
+        <v>2796</v>
       </c>
       <c r="D994" s="30" t="s">
+        <v>2797</v>
+      </c>
+      <c r="E994" s="39" t="s">
         <v>2796</v>
       </c>
-      <c r="E994" s="39" t="s">
-        <v>2795</v>
-      </c>
       <c r="F994" s="39" t="s">
-        <v>2795</v>
+        <v>2796</v>
       </c>
     </row>
     <row r="995" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30343,19 +30372,19 @@
         <v>991</v>
       </c>
       <c r="B995" s="1" t="s">
-        <v>2797</v>
+        <v>2798</v>
       </c>
       <c r="C995" s="1" t="s">
-        <v>2798</v>
+        <v>2799</v>
       </c>
       <c r="D995" s="1" t="s">
+        <v>2800</v>
+      </c>
+      <c r="E995" s="1" t="s">
         <v>2799</v>
       </c>
-      <c r="E995" s="1" t="s">
-        <v>2798</v>
-      </c>
       <c r="F995" s="1" t="s">
-        <v>2798</v>
+        <v>2799</v>
       </c>
     </row>
     <row r="996" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30363,19 +30392,19 @@
         <v>992</v>
       </c>
       <c r="B996" s="1" t="s">
-        <v>2800</v>
+        <v>2801</v>
       </c>
       <c r="C996" s="1" t="s">
-        <v>2801</v>
+        <v>2802</v>
       </c>
       <c r="D996" s="1" t="s">
+        <v>2803</v>
+      </c>
+      <c r="E996" s="1" t="s">
         <v>2802</v>
       </c>
-      <c r="E996" s="1" t="s">
-        <v>2801</v>
-      </c>
       <c r="F996" s="1" t="s">
-        <v>2801</v>
+        <v>2802</v>
       </c>
     </row>
     <row r="997" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30383,19 +30412,19 @@
         <v>993</v>
       </c>
       <c r="B997" s="1" t="s">
-        <v>2803</v>
+        <v>2804</v>
       </c>
       <c r="C997" s="1" t="s">
-        <v>2804</v>
+        <v>2805</v>
       </c>
       <c r="D997" s="1" t="s">
+        <v>2806</v>
+      </c>
+      <c r="E997" s="1" t="s">
         <v>2805</v>
       </c>
-      <c r="E997" s="1" t="s">
-        <v>2804</v>
-      </c>
       <c r="F997" s="1" t="s">
-        <v>2804</v>
+        <v>2805</v>
       </c>
     </row>
     <row r="998" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30403,19 +30432,19 @@
         <v>994</v>
       </c>
       <c r="B998" s="1" t="s">
-        <v>2806</v>
+        <v>2807</v>
       </c>
       <c r="C998" s="1" t="s">
-        <v>2807</v>
+        <v>2808</v>
       </c>
       <c r="D998" s="1" t="s">
+        <v>2809</v>
+      </c>
+      <c r="E998" s="1" t="s">
         <v>2808</v>
       </c>
-      <c r="E998" s="1" t="s">
-        <v>2807</v>
-      </c>
       <c r="F998" s="1" t="s">
-        <v>2807</v>
+        <v>2808</v>
       </c>
     </row>
     <row r="999" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30423,19 +30452,19 @@
         <v>995</v>
       </c>
       <c r="B999" s="1" t="s">
-        <v>2809</v>
+        <v>2810</v>
       </c>
       <c r="C999" s="1" t="s">
-        <v>2810</v>
+        <v>2811</v>
       </c>
       <c r="D999" s="1" t="s">
+        <v>2812</v>
+      </c>
+      <c r="E999" s="1" t="s">
         <v>2811</v>
       </c>
-      <c r="E999" s="1" t="s">
-        <v>2810</v>
-      </c>
       <c r="F999" s="1" t="s">
-        <v>2810</v>
+        <v>2811</v>
       </c>
     </row>
     <row r="1000" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30443,19 +30472,19 @@
         <v>996</v>
       </c>
       <c r="B1000" s="1" t="s">
-        <v>2812</v>
+        <v>2813</v>
       </c>
       <c r="C1000" s="1" t="s">
-        <v>2813</v>
+        <v>2814</v>
       </c>
       <c r="D1000" s="1" t="s">
+        <v>2815</v>
+      </c>
+      <c r="E1000" s="1" t="s">
         <v>2814</v>
       </c>
-      <c r="E1000" s="1" t="s">
-        <v>2813</v>
-      </c>
       <c r="F1000" s="1" t="s">
-        <v>2813</v>
+        <v>2814</v>
       </c>
     </row>
     <row r="1001" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30463,19 +30492,19 @@
         <v>997</v>
       </c>
       <c r="B1001" s="1" t="s">
-        <v>2815</v>
+        <v>2816</v>
       </c>
       <c r="C1001" s="1" t="s">
-        <v>2816</v>
+        <v>2817</v>
       </c>
       <c r="D1001" s="1" t="s">
+        <v>2818</v>
+      </c>
+      <c r="E1001" s="1" t="s">
         <v>2817</v>
       </c>
-      <c r="E1001" s="1" t="s">
-        <v>2816</v>
-      </c>
       <c r="F1001" s="1" t="s">
-        <v>2816</v>
+        <v>2817</v>
       </c>
     </row>
     <row r="1002" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30483,19 +30512,19 @@
         <v>998</v>
       </c>
       <c r="B1002" s="1" t="s">
-        <v>2818</v>
+        <v>2819</v>
       </c>
       <c r="C1002" s="1" t="s">
-        <v>2819</v>
+        <v>2820</v>
       </c>
       <c r="D1002" s="1" t="s">
+        <v>2821</v>
+      </c>
+      <c r="E1002" s="1" t="s">
         <v>2820</v>
       </c>
-      <c r="E1002" s="1" t="s">
-        <v>2819</v>
-      </c>
       <c r="F1002" s="1" t="s">
-        <v>2819</v>
+        <v>2820</v>
       </c>
     </row>
     <row r="1003" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30503,19 +30532,19 @@
         <v>999</v>
       </c>
       <c r="B1003" s="1" t="s">
-        <v>2821</v>
+        <v>2822</v>
       </c>
       <c r="C1003" s="1" t="s">
-        <v>2822</v>
+        <v>2823</v>
       </c>
       <c r="D1003" s="1" t="s">
+        <v>2824</v>
+      </c>
+      <c r="E1003" s="1" t="s">
         <v>2823</v>
       </c>
-      <c r="E1003" s="1" t="s">
-        <v>2822</v>
-      </c>
       <c r="F1003" s="1" t="s">
-        <v>2822</v>
+        <v>2823</v>
       </c>
     </row>
     <row r="1004" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30523,19 +30552,19 @@
         <v>1000</v>
       </c>
       <c r="B1004" s="1" t="s">
-        <v>2824</v>
+        <v>2825</v>
       </c>
       <c r="C1004" s="1" t="s">
-        <v>2825</v>
+        <v>2826</v>
       </c>
       <c r="D1004" s="1" t="s">
+        <v>2827</v>
+      </c>
+      <c r="E1004" s="1" t="s">
         <v>2826</v>
       </c>
-      <c r="E1004" s="1" t="s">
-        <v>2825</v>
-      </c>
       <c r="F1004" s="1" t="s">
-        <v>2825</v>
+        <v>2826</v>
       </c>
     </row>
     <row r="1005" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30543,19 +30572,19 @@
         <v>1001</v>
       </c>
       <c r="B1005" s="1" t="s">
-        <v>2827</v>
+        <v>2828</v>
       </c>
       <c r="C1005" s="1" t="s">
-        <v>2828</v>
+        <v>2829</v>
       </c>
       <c r="D1005" s="1" t="s">
+        <v>2830</v>
+      </c>
+      <c r="E1005" s="1" t="s">
         <v>2829</v>
       </c>
-      <c r="E1005" s="1" t="s">
-        <v>2828</v>
-      </c>
       <c r="F1005" s="1" t="s">
-        <v>2828</v>
+        <v>2829</v>
       </c>
     </row>
     <row r="1006" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30563,19 +30592,19 @@
         <v>1002</v>
       </c>
       <c r="B1006" s="1" t="s">
-        <v>2830</v>
+        <v>2831</v>
       </c>
       <c r="C1006" s="1" t="s">
-        <v>2831</v>
+        <v>2832</v>
       </c>
       <c r="D1006" s="1" t="s">
+        <v>2833</v>
+      </c>
+      <c r="E1006" s="1" t="s">
         <v>2832</v>
       </c>
-      <c r="E1006" s="1" t="s">
-        <v>2831</v>
-      </c>
       <c r="F1006" s="1" t="s">
-        <v>2831</v>
+        <v>2832</v>
       </c>
     </row>
     <row r="1007" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30583,19 +30612,19 @@
         <v>1003</v>
       </c>
       <c r="B1007" s="1" t="s">
-        <v>2833</v>
+        <v>2834</v>
       </c>
       <c r="C1007" s="1" t="s">
-        <v>2834</v>
+        <v>2835</v>
       </c>
       <c r="D1007" s="1" t="s">
+        <v>2836</v>
+      </c>
+      <c r="E1007" s="1" t="s">
         <v>2835</v>
       </c>
-      <c r="E1007" s="1" t="s">
-        <v>2834</v>
-      </c>
       <c r="F1007" s="1" t="s">
-        <v>2834</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="1008" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30603,19 +30632,19 @@
         <v>1004</v>
       </c>
       <c r="B1008" s="1" t="s">
-        <v>2836</v>
+        <v>2837</v>
       </c>
       <c r="C1008" s="1" t="s">
-        <v>2837</v>
+        <v>2838</v>
       </c>
       <c r="D1008" s="1" t="s">
+        <v>2839</v>
+      </c>
+      <c r="E1008" s="1" t="s">
         <v>2838</v>
       </c>
-      <c r="E1008" s="1" t="s">
-        <v>2837</v>
-      </c>
       <c r="F1008" s="1" t="s">
-        <v>2837</v>
+        <v>2838</v>
       </c>
     </row>
     <row r="1009" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30623,19 +30652,19 @@
         <v>1005</v>
       </c>
       <c r="B1009" s="1" t="s">
-        <v>2839</v>
+        <v>2840</v>
       </c>
       <c r="C1009" s="1" t="s">
-        <v>2840</v>
+        <v>2841</v>
       </c>
       <c r="D1009" s="1" t="s">
+        <v>2842</v>
+      </c>
+      <c r="E1009" s="1" t="s">
         <v>2841</v>
       </c>
-      <c r="E1009" s="1" t="s">
-        <v>2840</v>
-      </c>
       <c r="F1009" s="1" t="s">
-        <v>2840</v>
+        <v>2841</v>
       </c>
     </row>
     <row r="1010" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30643,19 +30672,19 @@
         <v>1006</v>
       </c>
       <c r="B1010" s="1" t="s">
-        <v>2842</v>
+        <v>2843</v>
       </c>
       <c r="C1010" s="1" t="s">
-        <v>2843</v>
+        <v>2844</v>
       </c>
       <c r="D1010" s="1" t="s">
+        <v>2845</v>
+      </c>
+      <c r="E1010" s="1" t="s">
         <v>2844</v>
       </c>
-      <c r="E1010" s="1" t="s">
-        <v>2843</v>
-      </c>
       <c r="F1010" s="1" t="s">
-        <v>2843</v>
+        <v>2844</v>
       </c>
     </row>
     <row r="1011" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30663,19 +30692,19 @@
         <v>1007</v>
       </c>
       <c r="B1011" s="1" t="s">
-        <v>2845</v>
+        <v>2846</v>
       </c>
       <c r="C1011" s="1" t="s">
-        <v>2846</v>
+        <v>2847</v>
       </c>
       <c r="D1011" s="1" t="s">
+        <v>2848</v>
+      </c>
+      <c r="E1011" s="1" t="s">
         <v>2847</v>
       </c>
-      <c r="E1011" s="1" t="s">
-        <v>2846</v>
-      </c>
       <c r="F1011" s="1" t="s">
-        <v>2846</v>
+        <v>2847</v>
       </c>
     </row>
     <row r="1012" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30683,19 +30712,19 @@
         <v>1008</v>
       </c>
       <c r="B1012" s="1" t="s">
-        <v>2848</v>
+        <v>2849</v>
       </c>
       <c r="C1012" s="1" t="s">
-        <v>2849</v>
+        <v>2850</v>
       </c>
       <c r="D1012" s="1" t="s">
+        <v>2851</v>
+      </c>
+      <c r="E1012" s="1" t="s">
         <v>2850</v>
       </c>
-      <c r="E1012" s="1" t="s">
-        <v>2849</v>
-      </c>
       <c r="F1012" s="1" t="s">
-        <v>2849</v>
+        <v>2850</v>
       </c>
     </row>
     <row r="1013" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30703,19 +30732,19 @@
         <v>1009</v>
       </c>
       <c r="B1013" s="1" t="s">
-        <v>2851</v>
+        <v>2852</v>
       </c>
       <c r="C1013" s="1" t="s">
-        <v>2852</v>
+        <v>2853</v>
       </c>
       <c r="D1013" s="1" t="s">
+        <v>2854</v>
+      </c>
+      <c r="E1013" s="1" t="s">
         <v>2853</v>
       </c>
-      <c r="E1013" s="1" t="s">
-        <v>2852</v>
-      </c>
       <c r="F1013" s="1" t="s">
-        <v>2852</v>
+        <v>2853</v>
       </c>
     </row>
     <row r="1014" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30723,19 +30752,19 @@
         <v>1010</v>
       </c>
       <c r="B1014" s="1" t="s">
-        <v>2854</v>
+        <v>2855</v>
       </c>
       <c r="C1014" s="1" t="s">
-        <v>2855</v>
+        <v>2856</v>
       </c>
       <c r="D1014" s="1" t="s">
+        <v>2857</v>
+      </c>
+      <c r="E1014" s="1" t="s">
         <v>2856</v>
       </c>
-      <c r="E1014" s="1" t="s">
-        <v>2855</v>
-      </c>
       <c r="F1014" s="1" t="s">
-        <v>2855</v>
+        <v>2856</v>
       </c>
     </row>
     <row r="1015" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30743,19 +30772,19 @@
         <v>1011</v>
       </c>
       <c r="B1015" s="1" t="s">
-        <v>2857</v>
+        <v>2858</v>
       </c>
       <c r="C1015" s="1" t="s">
-        <v>2858</v>
+        <v>2859</v>
       </c>
       <c r="D1015" s="1" t="s">
+        <v>2860</v>
+      </c>
+      <c r="E1015" s="1" t="s">
         <v>2859</v>
       </c>
-      <c r="E1015" s="1" t="s">
-        <v>2858</v>
-      </c>
       <c r="F1015" s="1" t="s">
-        <v>2858</v>
+        <v>2859</v>
       </c>
     </row>
     <row r="1016" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30763,19 +30792,19 @@
         <v>1012</v>
       </c>
       <c r="B1016" s="1" t="s">
-        <v>2860</v>
+        <v>2861</v>
       </c>
       <c r="C1016" s="1" t="s">
-        <v>2861</v>
+        <v>2862</v>
       </c>
       <c r="D1016" s="1" t="s">
+        <v>2863</v>
+      </c>
+      <c r="E1016" s="1" t="s">
         <v>2862</v>
       </c>
-      <c r="E1016" s="1" t="s">
-        <v>2861</v>
-      </c>
       <c r="F1016" s="1" t="s">
-        <v>2861</v>
+        <v>2862</v>
       </c>
     </row>
     <row r="1017" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30783,19 +30812,19 @@
         <v>1013</v>
       </c>
       <c r="B1017" s="1" t="s">
-        <v>2863</v>
+        <v>2864</v>
       </c>
       <c r="C1017" s="1" t="s">
-        <v>2864</v>
+        <v>2865</v>
       </c>
       <c r="D1017" s="1" t="s">
+        <v>2866</v>
+      </c>
+      <c r="E1017" s="1" t="s">
         <v>2865</v>
       </c>
-      <c r="E1017" s="1" t="s">
-        <v>2864</v>
-      </c>
       <c r="F1017" s="1" t="s">
-        <v>2864</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="1018" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30803,19 +30832,19 @@
         <v>1014</v>
       </c>
       <c r="B1018" s="1" t="s">
-        <v>2866</v>
+        <v>2867</v>
       </c>
       <c r="C1018" s="1" t="s">
-        <v>2867</v>
+        <v>2868</v>
       </c>
       <c r="D1018" s="1" t="s">
+        <v>2869</v>
+      </c>
+      <c r="E1018" s="1" t="s">
         <v>2868</v>
       </c>
-      <c r="E1018" s="1" t="s">
-        <v>2867</v>
-      </c>
       <c r="F1018" s="1" t="s">
-        <v>2867</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="1019" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30823,19 +30852,19 @@
         <v>1015</v>
       </c>
       <c r="B1019" s="1" t="s">
-        <v>2869</v>
+        <v>2870</v>
       </c>
       <c r="C1019" s="1" t="s">
-        <v>2870</v>
+        <v>2871</v>
       </c>
       <c r="D1019" s="1" t="s">
+        <v>2872</v>
+      </c>
+      <c r="E1019" s="1" t="s">
         <v>2871</v>
       </c>
-      <c r="E1019" s="1" t="s">
-        <v>2870</v>
-      </c>
       <c r="F1019" s="1" t="s">
-        <v>2870</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="1020" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30843,19 +30872,19 @@
         <v>1016</v>
       </c>
       <c r="B1020" s="1" t="s">
-        <v>2872</v>
+        <v>2873</v>
       </c>
       <c r="C1020" s="1" t="s">
-        <v>2873</v>
+        <v>2874</v>
       </c>
       <c r="D1020" s="1" t="s">
+        <v>2875</v>
+      </c>
+      <c r="E1020" s="1" t="s">
         <v>2874</v>
       </c>
-      <c r="E1020" s="1" t="s">
-        <v>2873</v>
-      </c>
       <c r="F1020" s="1" t="s">
-        <v>2873</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="1021" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30863,19 +30892,19 @@
         <v>1017</v>
       </c>
       <c r="B1021" s="1" t="s">
-        <v>2875</v>
+        <v>2876</v>
       </c>
       <c r="C1021" s="1" t="s">
-        <v>2876</v>
+        <v>2877</v>
       </c>
       <c r="D1021" s="1" t="s">
+        <v>2878</v>
+      </c>
+      <c r="E1021" s="1" t="s">
         <v>2877</v>
       </c>
-      <c r="E1021" s="1" t="s">
-        <v>2876</v>
-      </c>
       <c r="F1021" s="1" t="s">
-        <v>2876</v>
+        <v>2877</v>
       </c>
     </row>
     <row r="1022" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30883,19 +30912,19 @@
         <v>1018</v>
       </c>
       <c r="B1022" s="1" t="s">
-        <v>2878</v>
+        <v>2879</v>
       </c>
       <c r="C1022" s="1" t="s">
-        <v>2879</v>
+        <v>2880</v>
       </c>
       <c r="D1022" s="1" t="s">
+        <v>2881</v>
+      </c>
+      <c r="E1022" s="1" t="s">
         <v>2880</v>
       </c>
-      <c r="E1022" s="1" t="s">
-        <v>2879</v>
-      </c>
       <c r="F1022" s="1" t="s">
-        <v>2879</v>
+        <v>2880</v>
       </c>
     </row>
     <row r="1023" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30903,19 +30932,19 @@
         <v>1019</v>
       </c>
       <c r="B1023" s="1" t="s">
-        <v>2881</v>
+        <v>2882</v>
       </c>
       <c r="C1023" s="1" t="s">
-        <v>2882</v>
+        <v>2883</v>
       </c>
       <c r="D1023" s="1" t="s">
+        <v>2884</v>
+      </c>
+      <c r="E1023" s="1" t="s">
         <v>2883</v>
       </c>
-      <c r="E1023" s="1" t="s">
-        <v>2882</v>
-      </c>
       <c r="F1023" s="1" t="s">
-        <v>2882</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="1024" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30923,19 +30952,19 @@
         <v>1020</v>
       </c>
       <c r="B1024" s="1" t="s">
-        <v>2884</v>
+        <v>2885</v>
       </c>
       <c r="C1024" s="1" t="s">
-        <v>2885</v>
+        <v>2886</v>
       </c>
       <c r="D1024" s="1" t="s">
+        <v>2887</v>
+      </c>
+      <c r="E1024" s="1" t="s">
         <v>2886</v>
       </c>
-      <c r="E1024" s="1" t="s">
-        <v>2885</v>
-      </c>
       <c r="F1024" s="1" t="s">
-        <v>2885</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="1025" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30943,19 +30972,19 @@
         <v>1021</v>
       </c>
       <c r="B1025" s="1" t="s">
-        <v>2887</v>
+        <v>2888</v>
       </c>
       <c r="C1025" s="9" t="s">
-        <v>2888</v>
+        <v>2889</v>
       </c>
       <c r="D1025" s="1" t="s">
-        <v>2889</v>
+        <v>2890</v>
       </c>
       <c r="E1025" s="9" t="s">
-        <v>2890</v>
+        <v>2891</v>
       </c>
       <c r="F1025" s="9" t="s">
-        <v>2890</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="1026" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30963,19 +30992,19 @@
         <v>1022</v>
       </c>
       <c r="B1026" s="1" t="s">
-        <v>2891</v>
+        <v>2892</v>
       </c>
       <c r="C1026" s="9" t="s">
-        <v>2892</v>
+        <v>2893</v>
       </c>
       <c r="D1026" s="1" t="s">
-        <v>2893</v>
+        <v>2894</v>
       </c>
       <c r="E1026" s="9" t="s">
-        <v>2894</v>
+        <v>2895</v>
       </c>
       <c r="F1026" s="9" t="s">
-        <v>2894</v>
+        <v>2895</v>
       </c>
     </row>
     <row r="1027" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30983,19 +31012,19 @@
         <v>1023</v>
       </c>
       <c r="B1027" s="1" t="s">
-        <v>2895</v>
+        <v>2896</v>
       </c>
       <c r="C1027" s="9" t="s">
-        <v>2896</v>
+        <v>2897</v>
       </c>
       <c r="D1027" s="1" t="s">
+        <v>2898</v>
+      </c>
+      <c r="E1027" s="9" t="s">
         <v>2897</v>
       </c>
-      <c r="E1027" s="9" t="s">
-        <v>2896</v>
-      </c>
       <c r="F1027" s="9" t="s">
-        <v>2896</v>
+        <v>2897</v>
       </c>
     </row>
     <row r="1028" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31003,19 +31032,19 @@
         <v>1024</v>
       </c>
       <c r="B1028" s="1" t="s">
-        <v>2898</v>
+        <v>2899</v>
       </c>
       <c r="C1028" s="1" t="s">
-        <v>2899</v>
+        <v>2900</v>
       </c>
       <c r="D1028" s="1" t="s">
+        <v>2901</v>
+      </c>
+      <c r="E1028" s="1" t="s">
         <v>2900</v>
       </c>
-      <c r="E1028" s="1" t="s">
-        <v>2899</v>
-      </c>
       <c r="F1028" s="1" t="s">
-        <v>2899</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="1029" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31023,19 +31052,19 @@
         <v>1025</v>
       </c>
       <c r="B1029" s="1" t="s">
-        <v>2901</v>
+        <v>2902</v>
       </c>
       <c r="C1029" s="1" t="s">
-        <v>2902</v>
+        <v>2903</v>
       </c>
       <c r="D1029" s="1" t="s">
+        <v>2904</v>
+      </c>
+      <c r="E1029" s="1" t="s">
         <v>2903</v>
       </c>
-      <c r="E1029" s="1" t="s">
-        <v>2902</v>
-      </c>
       <c r="F1029" s="1" t="s">
-        <v>2902</v>
+        <v>2903</v>
       </c>
     </row>
     <row r="1030" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31043,19 +31072,19 @@
         <v>1026</v>
       </c>
       <c r="B1030" s="1" t="s">
-        <v>2904</v>
+        <v>2905</v>
       </c>
       <c r="C1030" s="1" t="s">
-        <v>2905</v>
+        <v>2906</v>
       </c>
       <c r="D1030" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="E1030" s="1" t="s">
         <v>2906</v>
       </c>
-      <c r="E1030" s="1" t="s">
-        <v>2905</v>
-      </c>
       <c r="F1030" s="1" t="s">
-        <v>2905</v>
+        <v>2906</v>
       </c>
     </row>
     <row r="1031" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31063,19 +31092,19 @@
         <v>1027</v>
       </c>
       <c r="B1031" s="1" t="s">
-        <v>2907</v>
+        <v>2908</v>
       </c>
       <c r="C1031" s="1" t="s">
-        <v>2908</v>
+        <v>2909</v>
       </c>
       <c r="D1031" s="1" t="s">
+        <v>2910</v>
+      </c>
+      <c r="E1031" s="1" t="s">
         <v>2909</v>
       </c>
-      <c r="E1031" s="1" t="s">
-        <v>2908</v>
-      </c>
       <c r="F1031" s="1" t="s">
-        <v>2908</v>
+        <v>2909</v>
       </c>
     </row>
     <row r="1032" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31083,19 +31112,19 @@
         <v>1028</v>
       </c>
       <c r="B1032" s="1" t="s">
-        <v>2910</v>
+        <v>2911</v>
       </c>
       <c r="C1032" s="1" t="s">
-        <v>2911</v>
+        <v>2912</v>
       </c>
       <c r="D1032" s="1" t="s">
+        <v>2913</v>
+      </c>
+      <c r="E1032" s="1" t="s">
         <v>2912</v>
       </c>
-      <c r="E1032" s="1" t="s">
-        <v>2911</v>
-      </c>
       <c r="F1032" s="1" t="s">
-        <v>2911</v>
+        <v>2912</v>
       </c>
     </row>
     <row r="1033" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31103,19 +31132,19 @@
         <v>1029</v>
       </c>
       <c r="B1033" s="1" t="s">
-        <v>2913</v>
+        <v>2914</v>
       </c>
       <c r="C1033" s="1" t="s">
-        <v>2914</v>
+        <v>2915</v>
       </c>
       <c r="D1033" s="1" t="s">
+        <v>2916</v>
+      </c>
+      <c r="E1033" s="1" t="s">
         <v>2915</v>
       </c>
-      <c r="E1033" s="1" t="s">
-        <v>2914</v>
-      </c>
       <c r="F1033" s="1" t="s">
-        <v>2914</v>
+        <v>2915</v>
       </c>
     </row>
     <row r="1034" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31123,19 +31152,19 @@
         <v>1030</v>
       </c>
       <c r="B1034" s="1" t="s">
-        <v>2916</v>
+        <v>2917</v>
       </c>
       <c r="C1034" s="1" t="s">
-        <v>2917</v>
+        <v>2918</v>
       </c>
       <c r="D1034" s="1" t="s">
+        <v>2919</v>
+      </c>
+      <c r="E1034" s="1" t="s">
         <v>2918</v>
       </c>
-      <c r="E1034" s="1" t="s">
-        <v>2917</v>
-      </c>
       <c r="F1034" s="1" t="s">
-        <v>2917</v>
+        <v>2918</v>
       </c>
     </row>
     <row r="1035" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31143,19 +31172,19 @@
         <v>1031</v>
       </c>
       <c r="B1035" s="1" t="s">
-        <v>2919</v>
+        <v>2920</v>
       </c>
       <c r="C1035" s="1" t="s">
-        <v>2920</v>
+        <v>2921</v>
       </c>
       <c r="D1035" s="1" t="s">
+        <v>2922</v>
+      </c>
+      <c r="E1035" s="1" t="s">
         <v>2921</v>
       </c>
-      <c r="E1035" s="1" t="s">
-        <v>2920</v>
-      </c>
       <c r="F1035" s="1" t="s">
-        <v>2920</v>
+        <v>2921</v>
       </c>
     </row>
     <row r="1036" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31163,19 +31192,19 @@
         <v>1032</v>
       </c>
       <c r="B1036" s="1" t="s">
-        <v>2922</v>
+        <v>2923</v>
       </c>
       <c r="C1036" s="1" t="s">
-        <v>2923</v>
+        <v>2924</v>
       </c>
       <c r="D1036" s="1" t="s">
+        <v>2925</v>
+      </c>
+      <c r="E1036" s="1" t="s">
         <v>2924</v>
       </c>
-      <c r="E1036" s="1" t="s">
-        <v>2923</v>
-      </c>
       <c r="F1036" s="1" t="s">
-        <v>2923</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="1037" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31183,19 +31212,19 @@
         <v>1033</v>
       </c>
       <c r="B1037" s="1" t="s">
-        <v>2925</v>
+        <v>2926</v>
       </c>
       <c r="C1037" s="1" t="s">
-        <v>2926</v>
+        <v>2927</v>
       </c>
       <c r="D1037" s="1" t="s">
+        <v>2928</v>
+      </c>
+      <c r="E1037" s="1" t="s">
         <v>2927</v>
       </c>
-      <c r="E1037" s="1" t="s">
-        <v>2926</v>
-      </c>
       <c r="F1037" s="1" t="s">
-        <v>2926</v>
+        <v>2927</v>
       </c>
     </row>
     <row r="1038" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31203,19 +31232,19 @@
         <v>1034</v>
       </c>
       <c r="B1038" s="1" t="s">
-        <v>2928</v>
+        <v>2929</v>
       </c>
       <c r="C1038" s="1" t="s">
-        <v>2929</v>
+        <v>2930</v>
       </c>
       <c r="D1038" s="1" t="s">
+        <v>2931</v>
+      </c>
+      <c r="E1038" s="1" t="s">
         <v>2930</v>
       </c>
-      <c r="E1038" s="1" t="s">
-        <v>2929</v>
-      </c>
       <c r="F1038" s="1" t="s">
-        <v>2929</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1040" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31223,19 +31252,19 @@
         <v>1035</v>
       </c>
       <c r="B1040" s="40" t="s">
-        <v>2931</v>
+        <v>2932</v>
       </c>
       <c r="C1040" s="9" t="s">
-        <v>2932</v>
+        <v>2933</v>
       </c>
       <c r="D1040" s="40" t="s">
+        <v>2934</v>
+      </c>
+      <c r="E1040" s="9" t="s">
         <v>2933</v>
       </c>
-      <c r="E1040" s="9" t="s">
-        <v>2932</v>
-      </c>
       <c r="F1040" s="9" t="s">
-        <v>2932</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1041" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31243,19 +31272,19 @@
         <v>1036</v>
       </c>
       <c r="B1041" s="40" t="s">
-        <v>2934</v>
+        <v>2935</v>
       </c>
       <c r="C1041" s="9" t="s">
-        <v>2935</v>
+        <v>2936</v>
       </c>
       <c r="D1041" s="40" t="s">
+        <v>2937</v>
+      </c>
+      <c r="E1041" s="9" t="s">
         <v>2936</v>
       </c>
-      <c r="E1041" s="9" t="s">
-        <v>2935</v>
-      </c>
       <c r="F1041" s="9" t="s">
-        <v>2935</v>
+        <v>2936</v>
       </c>
     </row>
     <row r="1042" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31263,19 +31292,19 @@
         <v>1037</v>
       </c>
       <c r="B1042" s="40" t="s">
-        <v>2937</v>
+        <v>2938</v>
       </c>
       <c r="C1042" s="40" t="s">
-        <v>2938</v>
+        <v>2939</v>
       </c>
       <c r="D1042" s="40" t="s">
+        <v>2940</v>
+      </c>
+      <c r="E1042" s="40" t="s">
         <v>2939</v>
       </c>
-      <c r="E1042" s="40" t="s">
-        <v>2938</v>
-      </c>
       <c r="F1042" s="40" t="s">
-        <v>2938</v>
+        <v>2939</v>
       </c>
     </row>
     <row r="1043" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31283,19 +31312,19 @@
         <v>1038</v>
       </c>
       <c r="B1043" s="40" t="s">
-        <v>2940</v>
+        <v>2941</v>
       </c>
       <c r="C1043" s="40" t="s">
-        <v>2941</v>
+        <v>2942</v>
       </c>
       <c r="D1043" s="40" t="s">
+        <v>2943</v>
+      </c>
+      <c r="E1043" s="40" t="s">
         <v>2942</v>
       </c>
-      <c r="E1043" s="40" t="s">
-        <v>2941</v>
-      </c>
       <c r="F1043" s="40" t="s">
-        <v>2941</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="1044" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31303,19 +31332,19 @@
         <v>1039</v>
       </c>
       <c r="B1044" s="40" t="s">
-        <v>2943</v>
+        <v>2944</v>
       </c>
       <c r="C1044" s="41" t="s">
-        <v>2944</v>
+        <v>2945</v>
       </c>
       <c r="D1044" s="40" t="s">
+        <v>2946</v>
+      </c>
+      <c r="E1044" s="41" t="s">
         <v>2945</v>
       </c>
-      <c r="E1044" s="41" t="s">
-        <v>2944</v>
-      </c>
       <c r="F1044" s="41" t="s">
-        <v>2944</v>
+        <v>2945</v>
       </c>
     </row>
     <row r="1045" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31323,13 +31352,13 @@
         <v>1040</v>
       </c>
       <c r="B1045" s="40" t="s">
-        <v>2946</v>
+        <v>2947</v>
       </c>
       <c r="C1045" s="40" t="s">
         <v>780</v>
       </c>
       <c r="D1045" s="40" t="s">
-        <v>2947</v>
+        <v>2948</v>
       </c>
       <c r="E1045" s="40" t="s">
         <v>780</v>
@@ -31343,19 +31372,19 @@
         <v>1041</v>
       </c>
       <c r="B1047" s="1" t="s">
-        <v>2948</v>
+        <v>2949</v>
       </c>
       <c r="C1047" s="1" t="s">
-        <v>2949</v>
+        <v>2950</v>
       </c>
       <c r="D1047" s="1" t="s">
+        <v>2951</v>
+      </c>
+      <c r="E1047" s="1" t="s">
         <v>2950</v>
       </c>
-      <c r="E1047" s="1" t="s">
-        <v>2949</v>
-      </c>
       <c r="F1047" s="1" t="s">
-        <v>2949</v>
+        <v>2950</v>
       </c>
     </row>
     <row r="1048" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31363,19 +31392,19 @@
         <v>1042</v>
       </c>
       <c r="B1048" s="9" t="s">
-        <v>2951</v>
+        <v>2952</v>
       </c>
       <c r="C1048" s="9" t="s">
-        <v>2952</v>
+        <v>2953</v>
       </c>
       <c r="D1048" s="9" t="s">
+        <v>2954</v>
+      </c>
+      <c r="E1048" s="9" t="s">
         <v>2953</v>
       </c>
-      <c r="E1048" s="9" t="s">
-        <v>2952</v>
-      </c>
       <c r="F1048" s="9" t="s">
-        <v>2952</v>
+        <v>2953</v>
       </c>
     </row>
     <row r="1049" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31383,19 +31412,19 @@
         <v>1043</v>
       </c>
       <c r="B1049" s="1" t="s">
-        <v>2954</v>
+        <v>2955</v>
       </c>
       <c r="C1049" s="1" t="s">
-        <v>2955</v>
+        <v>2956</v>
       </c>
       <c r="D1049" s="1" t="s">
+        <v>2957</v>
+      </c>
+      <c r="E1049" s="1" t="s">
         <v>2956</v>
       </c>
-      <c r="E1049" s="1" t="s">
-        <v>2955</v>
-      </c>
       <c r="F1049" s="1" t="s">
-        <v>2955</v>
+        <v>2956</v>
       </c>
     </row>
     <row r="1050" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31403,19 +31432,19 @@
         <v>1044</v>
       </c>
       <c r="B1050" s="1" t="s">
-        <v>2957</v>
+        <v>2958</v>
       </c>
       <c r="C1050" s="1" t="s">
-        <v>2958</v>
+        <v>2959</v>
       </c>
       <c r="D1050" s="1" t="s">
+        <v>2960</v>
+      </c>
+      <c r="E1050" s="1" t="s">
         <v>2959</v>
       </c>
-      <c r="E1050" s="1" t="s">
-        <v>2958</v>
-      </c>
       <c r="F1050" s="1" t="s">
-        <v>2958</v>
+        <v>2959</v>
       </c>
     </row>
     <row r="1051" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31423,19 +31452,19 @@
         <v>1045</v>
       </c>
       <c r="B1051" s="1" t="s">
-        <v>2960</v>
+        <v>2961</v>
       </c>
       <c r="C1051" s="1" t="s">
-        <v>2961</v>
+        <v>2962</v>
       </c>
       <c r="D1051" s="1" t="s">
+        <v>2963</v>
+      </c>
+      <c r="E1051" s="1" t="s">
         <v>2962</v>
       </c>
-      <c r="E1051" s="1" t="s">
-        <v>2961</v>
-      </c>
       <c r="F1051" s="1" t="s">
-        <v>2961</v>
+        <v>2962</v>
       </c>
     </row>
     <row r="1052" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31443,19 +31472,19 @@
         <v>1046</v>
       </c>
       <c r="B1052" s="9" t="s">
-        <v>2963</v>
+        <v>2964</v>
       </c>
       <c r="C1052" s="9" t="s">
-        <v>2964</v>
+        <v>2965</v>
       </c>
       <c r="D1052" s="9" t="s">
+        <v>2966</v>
+      </c>
+      <c r="E1052" s="9" t="s">
         <v>2965</v>
       </c>
-      <c r="E1052" s="9" t="s">
-        <v>2964</v>
-      </c>
       <c r="F1052" s="9" t="s">
-        <v>2964</v>
+        <v>2965</v>
       </c>
     </row>
     <row r="1053" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31463,19 +31492,19 @@
         <v>1047</v>
       </c>
       <c r="B1053" s="9" t="s">
-        <v>2966</v>
+        <v>2967</v>
       </c>
       <c r="C1053" s="1" t="s">
-        <v>2967</v>
+        <v>2968</v>
       </c>
       <c r="D1053" s="1" t="s">
+        <v>2969</v>
+      </c>
+      <c r="E1053" s="1" t="s">
         <v>2968</v>
       </c>
-      <c r="E1053" s="1" t="s">
-        <v>2967</v>
-      </c>
       <c r="F1053" s="1" t="s">
-        <v>2967</v>
+        <v>2968</v>
       </c>
     </row>
     <row r="1054" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31483,19 +31512,19 @@
         <v>1048</v>
       </c>
       <c r="B1054" s="9" t="s">
-        <v>2969</v>
+        <v>2970</v>
       </c>
       <c r="C1054" s="1" t="s">
-        <v>2970</v>
+        <v>2971</v>
       </c>
       <c r="D1054" s="1" t="s">
+        <v>2972</v>
+      </c>
+      <c r="E1054" s="1" t="s">
         <v>2971</v>
       </c>
-      <c r="E1054" s="1" t="s">
-        <v>2970</v>
-      </c>
       <c r="F1054" s="1" t="s">
-        <v>2970</v>
+        <v>2971</v>
       </c>
     </row>
     <row r="1055" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31503,19 +31532,19 @@
         <v>1049</v>
       </c>
       <c r="B1055" s="9" t="s">
-        <v>2972</v>
+        <v>2973</v>
       </c>
       <c r="C1055" s="1" t="s">
-        <v>2973</v>
+        <v>2974</v>
       </c>
       <c r="D1055" s="1" t="s">
+        <v>2975</v>
+      </c>
+      <c r="E1055" s="1" t="s">
         <v>2974</v>
       </c>
-      <c r="E1055" s="1" t="s">
-        <v>2973</v>
-      </c>
       <c r="F1055" s="1" t="s">
-        <v>2973</v>
+        <v>2974</v>
       </c>
     </row>
     <row r="1056" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31523,19 +31552,19 @@
         <v>1050</v>
       </c>
       <c r="B1056" s="9" t="s">
-        <v>2975</v>
+        <v>2976</v>
       </c>
       <c r="C1056" s="1" t="s">
-        <v>2976</v>
+        <v>2977</v>
       </c>
       <c r="D1056" s="1" t="s">
+        <v>2978</v>
+      </c>
+      <c r="E1056" s="1" t="s">
         <v>2977</v>
       </c>
-      <c r="E1056" s="1" t="s">
-        <v>2976</v>
-      </c>
       <c r="F1056" s="1" t="s">
-        <v>2976</v>
+        <v>2977</v>
       </c>
     </row>
     <row r="1057" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31543,19 +31572,19 @@
         <v>1051</v>
       </c>
       <c r="B1057" s="9" t="s">
-        <v>2978</v>
+        <v>2979</v>
       </c>
       <c r="C1057" s="1" t="s">
-        <v>2979</v>
+        <v>2980</v>
       </c>
       <c r="D1057" s="1" t="s">
+        <v>2981</v>
+      </c>
+      <c r="E1057" s="1" t="s">
         <v>2980</v>
       </c>
-      <c r="E1057" s="1" t="s">
-        <v>2979</v>
-      </c>
       <c r="F1057" s="1" t="s">
-        <v>2979</v>
+        <v>2980</v>
       </c>
     </row>
     <row r="1058" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31563,19 +31592,19 @@
         <v>1052</v>
       </c>
       <c r="B1058" s="9" t="s">
-        <v>2981</v>
+        <v>2982</v>
       </c>
       <c r="C1058" s="1" t="s">
-        <v>2982</v>
+        <v>2983</v>
       </c>
       <c r="D1058" s="1" t="s">
+        <v>2984</v>
+      </c>
+      <c r="E1058" s="1" t="s">
         <v>2983</v>
       </c>
-      <c r="E1058" s="1" t="s">
-        <v>2982</v>
-      </c>
       <c r="F1058" s="1" t="s">
-        <v>2982</v>
+        <v>2983</v>
       </c>
     </row>
     <row r="1059" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31583,19 +31612,19 @@
         <v>1053</v>
       </c>
       <c r="B1059" s="9" t="s">
-        <v>2984</v>
+        <v>2985</v>
       </c>
       <c r="C1059" s="9" t="s">
-        <v>2985</v>
+        <v>2986</v>
       </c>
       <c r="D1059" s="9" t="s">
+        <v>2987</v>
+      </c>
+      <c r="E1059" s="9" t="s">
         <v>2986</v>
       </c>
-      <c r="E1059" s="9" t="s">
-        <v>2985</v>
-      </c>
       <c r="F1059" s="9" t="s">
-        <v>2985</v>
+        <v>2986</v>
       </c>
     </row>
     <row r="1060" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31603,19 +31632,19 @@
         <v>1054</v>
       </c>
       <c r="B1060" s="1" t="s">
-        <v>2987</v>
+        <v>2988</v>
       </c>
       <c r="C1060" s="42" t="s">
-        <v>2988</v>
+        <v>2989</v>
       </c>
       <c r="D1060" s="1" t="s">
+        <v>2990</v>
+      </c>
+      <c r="E1060" s="42" t="s">
         <v>2989</v>
       </c>
-      <c r="E1060" s="42" t="s">
-        <v>2988</v>
-      </c>
       <c r="F1060" s="42" t="s">
-        <v>2988</v>
+        <v>2989</v>
       </c>
     </row>
     <row r="1061" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31623,10 +31652,10 @@
         <v>1055</v>
       </c>
       <c r="B1061" s="1" t="s">
-        <v>2990</v>
+        <v>2991</v>
       </c>
       <c r="D1061" s="30" t="s">
-        <v>2991</v>
+        <v>2992</v>
       </c>
     </row>
     <row r="1062" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31634,10 +31663,10 @@
         <v>1056</v>
       </c>
       <c r="B1062" s="1" t="s">
-        <v>2992</v>
+        <v>2993</v>
       </c>
       <c r="D1062" s="30" t="s">
-        <v>2993</v>
+        <v>2994</v>
       </c>
     </row>
     <row r="1063" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31645,10 +31674,10 @@
         <v>1057</v>
       </c>
       <c r="B1063" s="1" t="s">
-        <v>2994</v>
+        <v>2995</v>
       </c>
       <c r="D1063" s="1" t="s">
-        <v>2995</v>
+        <v>2996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update：online shop type change
修改online shop ui 选中框格式修改
增加online shop 多语言
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/Language_多语言表.xlsx
+++ b/pet-simulator/Excel/Language_多语言表.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5337" uniqueCount="3010">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5357" uniqueCount="3020">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -9104,6 +9104,36 @@
   </si>
   <si>
     <t xml:space="preserve">尚未附魔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online_shop001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">仙豆</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online_shop002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test English Test English Test English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">在游戏中使用可获得60%体力</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online_shop003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">精灵球</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online_shop004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">在奖励地图中捕获龙娘时使用</t>
   </si>
 </sst>
 </file>
@@ -9710,10 +9740,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T1066"/>
+  <dimension ref="A1:T1070"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1049" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1069" activeCellId="0" sqref="D1069"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1055" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1079" activeCellId="0" sqref="F1079"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.12890625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31757,6 +31787,86 @@
       </c>
       <c r="E1066" s="1" t="s">
         <v>3008</v>
+      </c>
+    </row>
+    <row r="1067" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1067" s="1" t="n">
+        <v>1061</v>
+      </c>
+      <c r="B1067" s="1" t="s">
+        <v>3010</v>
+      </c>
+      <c r="C1067" s="1" t="s">
+        <v>3011</v>
+      </c>
+      <c r="D1067" s="1" t="s">
+        <v>3012</v>
+      </c>
+      <c r="E1067" s="1" t="s">
+        <v>3011</v>
+      </c>
+      <c r="F1067" s="1" t="s">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="1068" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1068" s="1" t="n">
+        <v>1062</v>
+      </c>
+      <c r="B1068" s="1" t="s">
+        <v>3013</v>
+      </c>
+      <c r="C1068" s="1" t="s">
+        <v>3014</v>
+      </c>
+      <c r="D1068" s="1" t="s">
+        <v>3015</v>
+      </c>
+      <c r="E1068" s="1" t="s">
+        <v>3014</v>
+      </c>
+      <c r="F1068" s="1" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="1069" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1069" s="1" t="n">
+        <v>1063</v>
+      </c>
+      <c r="B1069" s="1" t="s">
+        <v>3016</v>
+      </c>
+      <c r="C1069" s="1" t="s">
+        <v>3011</v>
+      </c>
+      <c r="D1069" s="1" t="s">
+        <v>3017</v>
+      </c>
+      <c r="E1069" s="1" t="s">
+        <v>3011</v>
+      </c>
+      <c r="F1069" s="1" t="s">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="1070" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1070" s="1" t="n">
+        <v>1064</v>
+      </c>
+      <c r="B1070" s="1" t="s">
+        <v>3018</v>
+      </c>
+      <c r="C1070" s="1" t="s">
+        <v>3014</v>
+      </c>
+      <c r="D1070" s="1" t="s">
+        <v>3019</v>
+      </c>
+      <c r="E1070" s="1" t="s">
+        <v>3014</v>
+      </c>
+      <c r="F1070" s="1" t="s">
+        <v>3014</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: update ps onlineshopUI
更新在线商店多语言
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/Language_多语言表.xlsx
+++ b/pet-simulator/Excel/Language_多语言表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Project\Edit\DragonVerse\pet-simulator\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B3EED2-501F-4C75-A47C-5805A26E855E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13374022-1E9C-4C37-9A59-511B167F063F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="译文-1" sheetId="1" r:id="rId1"/>
     <sheet name="WpsReserved_CellImgList" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -9805,8 +9805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1081"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A409" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D430" sqref="D430"/>
+    <sheetView tabSelected="1" topLeftCell="A306" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D332" sqref="D332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.125" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>

</xml_diff>